<commit_message>
Drag Update. Version: Perf Report
</commit_message>
<xml_diff>
--- a/Wing Tail Drag Buildup/Drag.xlsx
+++ b/Wing Tail Drag Buildup/Drag.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e\Documents\GitHub\Senior-Design\Wing Tail Drag Buildup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EddieH\Documents\GitHub\Senior-Design\Wing Tail Drag Buildup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E71467-A482-45DE-B487-F4277777C2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A673F954-7712-4AFC-B89B-A7C459871A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1470" windowWidth="28455" windowHeight="16620" xr2:uid="{82617F0D-A785-403D-9CC0-085A46D2A0AD}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{82617F0D-A785-403D-9CC0-085A46D2A0AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -727,18 +727,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470D6C11-8322-4BAC-B928-8395D64AAF23}">
   <dimension ref="A1:W30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.73046875" customWidth="1"/>
+    <col min="2" max="2" width="10.3984375" customWidth="1"/>
+    <col min="3" max="22" width="10.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
       <c r="I1" s="3" t="s">
         <v>30</v>
       </c>
@@ -761,7 +761,7 @@
       <c r="R1" s="8"/>
       <c r="S1" s="9"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
       <c r="I2" s="3" t="s">
         <v>27</v>
       </c>
@@ -779,7 +779,7 @@
       <c r="R2" s="11"/>
       <c r="S2" s="12"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -830,7 +830,7 @@
       </c>
       <c r="S3" s="12"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
       <c r="I4" s="3" t="s">
         <v>12</v>
       </c>
@@ -859,7 +859,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -904,15 +904,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>1459</v>
-      </c>
-      <c r="C6">
-        <v>694</v>
-      </c>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
       <c r="D6">
-        <v>2219.4</v>
+        <v>438</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -947,7 +941,7 @@
       </c>
       <c r="S6" s="15"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
       <c r="I7" t="s">
         <v>24</v>
       </c>
@@ -958,7 +952,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
       <c r="I8" t="s">
         <v>25</v>
       </c>
@@ -969,7 +963,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
       <c r="I9" s="3" t="s">
         <v>36</v>
       </c>
@@ -977,7 +971,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>51</v>
       </c>
@@ -985,7 +979,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1011,7 +1005,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1038,7 +1032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -1060,7 +1054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -1081,7 +1075,7 @@
         <v>0.1026</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>49</v>
       </c>
@@ -1095,7 +1089,7 @@
         <v>2.8163</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>50</v>
       </c>
@@ -1110,7 +1104,7 @@
         <v>11.547000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.45">
       <c r="H17" t="s">
         <v>54</v>
       </c>
@@ -1118,7 +1112,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1186,7 +1180,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1276,517 +1270,516 @@
       </c>
       <c r="W21" s="22"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A22" s="18" t="s">
         <v>46</v>
       </c>
       <c r="B22">
-        <v>7.0510000000000002</v>
+        <v>12.125500000000001</v>
       </c>
       <c r="C22">
-        <v>4.1769999999999996</v>
+        <v>8.9417500000000008</v>
       </c>
       <c r="D22">
-        <v>2.9769999999999999</v>
+        <v>6.0397499999999997</v>
       </c>
       <c r="E22">
-        <v>1.843</v>
+        <v>5.5709999999999997</v>
       </c>
       <c r="F22">
-        <v>1.0529999999999999</v>
+        <v>3.07775</v>
       </c>
       <c r="G22">
-        <v>0.48099999999999998</v>
+        <v>2.1127500000000001</v>
       </c>
       <c r="H22">
-        <v>4.4999999999999998E-2</v>
+        <v>1.4067499999999999</v>
       </c>
       <c r="I22">
-        <v>-0.29099999999999998</v>
+        <v>1.0002500000000001</v>
       </c>
       <c r="J22">
-        <v>-0.55300000000000005</v>
+        <v>0.43325000000000002</v>
       </c>
       <c r="K22">
-        <v>-0.76500000000000001</v>
+        <v>8.8749999999999996E-2</v>
       </c>
       <c r="L22">
-        <v>-0.93799999999999994</v>
+        <v>-0.1915</v>
       </c>
       <c r="M22">
-        <v>-1.08</v>
+        <v>-0.42099999999999999</v>
       </c>
       <c r="N22">
-        <v>-1.1990000000000001</v>
+        <v>-0.61575000000000002</v>
       </c>
       <c r="O22">
-        <v>-1.2989999999999999</v>
+        <v>-0.77875000000000005</v>
       </c>
       <c r="P22">
-        <v>-1.3839999999999999</v>
+        <v>-0.91725000000000001</v>
       </c>
       <c r="Q22">
-        <v>-1.456</v>
+        <v>-1.0369999999999999</v>
       </c>
       <c r="R22">
-        <v>-1.52</v>
+        <v>-1.14025</v>
       </c>
       <c r="S22">
-        <v>-1.575</v>
+        <v>-1.2297499999999999</v>
       </c>
       <c r="T22">
-        <v>-1.6220000000000001</v>
+        <v>-1.30775</v>
       </c>
       <c r="U22">
-        <v>-1.663</v>
+        <v>-1.3765000000000001</v>
       </c>
       <c r="V22">
-        <v>-1.7010000000000001</v>
+        <v>-1.4377500000000001</v>
       </c>
       <c r="W22" s="23" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A23" s="16" t="s">
         <v>35</v>
       </c>
       <c r="B23" s="2">
-        <f xml:space="preserve"> $D$6/(0.5*$J$3*B21^2*$J$4)</f>
-        <v>8.2924605554335695</v>
+        <v>1.5</v>
       </c>
       <c r="C23" s="2">
-        <f xml:space="preserve"> $D$6/(0.5*$J$3*C21^2*$J$4)</f>
-        <v>6.0924199999103781</v>
+        <f t="shared" ref="B23:V23" si="3" xml:space="preserve"> $D$6/(0.5*$J$3*C21^2*$J$4)</f>
+        <v>1.2023429575384093</v>
       </c>
       <c r="D23" s="2">
-        <f xml:space="preserve"> $D$6/(0.5*$J$3*D21^2*$J$4)</f>
-        <v>4.6645090624313816</v>
+        <f t="shared" si="3"/>
+        <v>0.92054382686534431</v>
       </c>
       <c r="E23" s="2">
-        <f xml:space="preserve"> $D$6/(0.5*$J$3*E21^2*$J$4)</f>
-        <v>3.6855380246371414</v>
+        <f t="shared" si="3"/>
+        <v>0.72734327060965487</v>
       </c>
       <c r="F23" s="2">
-        <f xml:space="preserve"> $D$6/(0.5*$J$3*F21^2*$J$4)</f>
-        <v>2.9852857999560842</v>
+        <f t="shared" si="3"/>
+        <v>0.58914804919382036</v>
       </c>
       <c r="G23" s="2">
-        <f xml:space="preserve"> $D$6/(0.5*$J$3*G21^2*$J$4)</f>
-        <v>2.4671783470711444</v>
+        <f t="shared" si="3"/>
+        <v>0.48689921420976895</v>
       </c>
       <c r="H23" s="2">
-        <f xml:space="preserve"> $D$6/(0.5*$J$3*H21^2*$J$4)</f>
-        <v>2.0731151388583924</v>
+        <f t="shared" si="3"/>
+        <v>0.40913058971793093</v>
       </c>
       <c r="I23" s="2">
-        <f xml:space="preserve"> $D$6/(0.5*$J$3*I21^2*$J$4)</f>
-        <v>1.7664413017491629</v>
+        <f t="shared" si="3"/>
+        <v>0.34860831313243817</v>
       </c>
       <c r="J23" s="2">
-        <f xml:space="preserve"> $D$6/(0.5*$J$3*J21^2*$J$4)</f>
-        <v>1.5231049999775945</v>
+        <f t="shared" si="3"/>
+        <v>0.30058573938460231</v>
       </c>
       <c r="K23" s="2">
-        <f xml:space="preserve"> $D$6/(0.5*$J$3*K21^2*$J$4)</f>
-        <v>1.3267936888693708</v>
+        <f t="shared" si="3"/>
+        <v>0.26184357741947573</v>
       </c>
       <c r="L23" s="2">
-        <f xml:space="preserve"> $D$6/(0.5*$J$3*L21^2*$J$4)</f>
-        <v>1.1661272656078454</v>
+        <f t="shared" si="3"/>
+        <v>0.23013595671633608</v>
       </c>
       <c r="M23" s="2">
-        <f xml:space="preserve"> $D$6/(0.5*$J$3*M21^2*$J$4)</f>
-        <v>1.0329708650367073</v>
+        <f t="shared" si="3"/>
+        <v>0.20385745646844994</v>
       </c>
       <c r="N23" s="2">
-        <f xml:space="preserve"> $D$6/(0.5*$J$3*N21^2*$J$4)</f>
-        <v>0.92138450615928535</v>
+        <f t="shared" si="3"/>
+        <v>0.18183581765241372</v>
       </c>
       <c r="O23" s="2">
-        <f xml:space="preserve"> $D$6/(0.5*$J$3*O21^2*$J$4)</f>
-        <v>0.82694897505708731</v>
+        <f t="shared" si="3"/>
+        <v>0.16319890559385608</v>
       </c>
       <c r="P23" s="2">
-        <f xml:space="preserve"> $D$6/(0.5*$J$3*P21^2*$J$4)</f>
-        <v>0.74632144998902106</v>
+        <f t="shared" si="3"/>
+        <v>0.14728701229845509</v>
       </c>
       <c r="Q23" s="2">
-        <f xml:space="preserve"> $D$6/(0.5*$J$3*Q21^2*$J$4)</f>
-        <v>0.67693555554559748</v>
+        <f t="shared" si="3"/>
+        <v>0.13359366194871211</v>
       </c>
       <c r="R23" s="2">
-        <f xml:space="preserve"> $D$6/(0.5*$J$3*R21^2*$J$4)</f>
-        <v>0.61679458676778609</v>
+        <f t="shared" si="3"/>
+        <v>0.12172480355244224</v>
       </c>
       <c r="S23" s="2">
-        <f xml:space="preserve"> $D$6/(0.5*$J$3*S21^2*$J$4)</f>
-        <v>0.5643262381769536</v>
+        <f t="shared" si="3"/>
+        <v>0.11137014162454073</v>
       </c>
       <c r="T23" s="2">
-        <f xml:space="preserve"> $D$6/(0.5*$J$3*T21^2*$J$4)</f>
-        <v>0.5182787847145981</v>
+        <f t="shared" si="3"/>
+        <v>0.10228264742948273</v>
       </c>
       <c r="U23" s="2">
-        <f xml:space="preserve"> $D$6/(0.5*$J$3*U21^2*$J$4)</f>
-        <v>0.47764572799297356</v>
+        <f t="shared" si="3"/>
+        <v>9.4263687871011262E-2</v>
       </c>
       <c r="V23" s="2">
-        <f xml:space="preserve"> $D$6/(0.5*$J$3*V21^2*$J$4)</f>
-        <v>0.44161032543729073</v>
+        <f t="shared" si="3"/>
+        <v>8.7152078283109544E-2</v>
       </c>
       <c r="W23" s="23" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A24" s="19" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="2">
-        <f>((1+$B$11)*(B23^2))/(PI()*$J$9)</f>
-        <v>1.5176060050144764</v>
+        <f t="shared" ref="B24:V24" si="4">((1+$B$11)*(B23^2))/(PI()*$J$9)</f>
+        <v>4.9656342244671345E-2</v>
       </c>
       <c r="C24" s="2">
-        <f>((1+$B$11)*(C23^2))/(PI()*$J$9)</f>
-        <v>0.81916592357299522</v>
+        <f t="shared" si="4"/>
+        <v>3.1904279067411896E-2</v>
       </c>
       <c r="D24" s="2">
-        <f>((1+$B$11)*(D23^2))/(PI()*$J$9)</f>
-        <v>0.48018002502411133</v>
+        <f t="shared" si="4"/>
+        <v>1.8701702646693338E-2</v>
       </c>
       <c r="E24" s="2">
-        <f>((1+$B$11)*(E23^2))/(PI()*$J$9)</f>
-        <v>0.29977402568187173</v>
+        <f t="shared" si="4"/>
+        <v>1.1675380893286992E-2</v>
       </c>
       <c r="F24" s="2">
-        <f>((1+$B$11)*(F23^2))/(PI()*$J$9)</f>
-        <v>0.196681738249876</v>
+        <f t="shared" si="4"/>
+        <v>7.6602174040855918E-3</v>
       </c>
       <c r="G24" s="2">
-        <f>((1+$B$11)*(G23^2))/(PI()*$J$9)</f>
-        <v>0.13433627364925627</v>
+        <f t="shared" si="4"/>
+        <v>5.2320315580121537E-3</v>
       </c>
       <c r="H24" s="2">
-        <f>((1+$B$11)*(H23^2))/(PI()*$J$9)</f>
-        <v>9.4850375313404775E-2</v>
+        <f t="shared" si="4"/>
+        <v>3.6941634857665879E-3</v>
       </c>
       <c r="I24" s="2">
-        <f>((1+$B$11)*(I23^2))/(PI()*$J$9)</f>
-        <v>6.8863743653890322E-2</v>
+        <f t="shared" si="4"/>
+        <v>2.6820550415201138E-3</v>
       </c>
       <c r="J24" s="2">
-        <f>((1+$B$11)*(J23^2))/(PI()*$J$9)</f>
-        <v>5.1197870223312202E-2</v>
+        <f t="shared" si="4"/>
+        <v>1.9940174417132435E-3</v>
       </c>
       <c r="K24" s="2">
-        <f>((1+$B$11)*(K23^2))/(PI()*$J$9)</f>
-        <v>3.8850713728370567E-2</v>
+        <f t="shared" si="4"/>
+        <v>1.5131293637699937E-3</v>
       </c>
       <c r="L24" s="2">
-        <f>((1+$B$11)*(L23^2))/(PI()*$J$9)</f>
-        <v>3.0011251564006958E-2</v>
+        <f t="shared" si="4"/>
+        <v>1.1688564154183336E-3</v>
       </c>
       <c r="M24" s="2">
-        <f>((1+$B$11)*(M23^2))/(PI()*$J$9)</f>
-        <v>2.3548776744755931E-2</v>
+        <f t="shared" si="4"/>
+        <v>9.1716064272285918E-4</v>
       </c>
       <c r="N24" s="2">
-        <f>((1+$B$11)*(N23^2))/(PI()*$J$9)</f>
-        <v>1.8735876605116983E-2</v>
+        <f t="shared" si="4"/>
+        <v>7.29711305830437E-4</v>
       </c>
       <c r="O24" s="2">
-        <f>((1+$B$11)*(O23^2))/(PI()*$J$9)</f>
-        <v>1.5092098606508248E-2</v>
+        <f t="shared" si="4"/>
+        <v>5.8779608843437324E-4</v>
       </c>
       <c r="P24" s="2">
-        <f>((1+$B$11)*(P23^2))/(PI()*$J$9)</f>
-        <v>1.229260864061725E-2</v>
+        <f t="shared" si="4"/>
+        <v>4.7876358775534949E-4</v>
       </c>
       <c r="Q24" s="2">
-        <f>((1+$B$11)*(Q23^2))/(PI()*$J$9)</f>
-        <v>1.011315955028389E-2</v>
+        <f t="shared" si="4"/>
+        <v>3.938799884865665E-4</v>
       </c>
       <c r="R24" s="2">
-        <f>((1+$B$11)*(R23^2))/(PI()*$J$9)</f>
-        <v>8.3960171030785166E-3</v>
+        <f t="shared" si="4"/>
+        <v>3.270019723757596E-4</v>
       </c>
       <c r="S24" s="2">
-        <f>((1+$B$11)*(S23^2))/(PI()*$J$9)</f>
-        <v>7.0283388870778785E-3</v>
+        <f t="shared" si="4"/>
+        <v>2.7373463517088613E-4</v>
       </c>
       <c r="T24" s="2">
-        <f>((1+$B$11)*(T23^2))/(PI()*$J$9)</f>
-        <v>5.9281484570877984E-3</v>
+        <f t="shared" si="4"/>
+        <v>2.3088521786041174E-4</v>
       </c>
       <c r="U24" s="2">
-        <f>((1+$B$11)*(U23^2))/(PI()*$J$9)</f>
-        <v>5.0350524991968279E-3</v>
+        <f t="shared" si="4"/>
+        <v>1.961015655445912E-4</v>
       </c>
       <c r="V24" s="2">
-        <f>((1+$B$11)*(V23^2))/(PI()*$J$9)</f>
-        <v>4.3039839783681451E-3</v>
+        <f t="shared" si="4"/>
+        <v>1.6762844009500711E-4</v>
       </c>
       <c r="W24" s="23" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A25" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="2">
-        <v>3.7677342669161298E-2</v>
+        <v>2.62996909074374E-2</v>
       </c>
       <c r="C25" s="2">
-        <v>2.44899992541599E-2</v>
+        <v>1.86289773519932E-2</v>
       </c>
       <c r="D25" s="2">
-        <v>2.0250215248781601E-2</v>
+        <v>1.2843480112571399E-2</v>
       </c>
       <c r="E25" s="2">
-        <v>1.9775066989825198E-2</v>
+        <v>9.8121395203986297E-3</v>
       </c>
       <c r="F25" s="2">
-        <v>2.0100102247298302E-2</v>
+        <v>8.1758070473596806E-3</v>
       </c>
       <c r="G25" s="2">
-        <v>2.0651940529969302E-2</v>
+        <v>7.9749493381566297E-3</v>
       </c>
       <c r="H25" s="2">
-        <v>2.10200900496849E-2</v>
+        <v>8.0370514870199104E-3</v>
       </c>
       <c r="I25" s="2">
-        <v>2.11462672638787E-2</v>
+        <v>8.1974836499532893E-3</v>
       </c>
       <c r="J25" s="2">
-        <v>2.1214944867359298E-2</v>
+        <v>8.3653514057388592E-3</v>
       </c>
       <c r="K25" s="2">
-        <v>2.1241298109474799E-2</v>
+        <v>8.4348891474543292E-3</v>
       </c>
       <c r="L25" s="2">
-        <v>2.13107775518812E-2</v>
+        <v>8.4772608253743907E-3</v>
       </c>
       <c r="M25" s="2">
-        <v>2.1283123476863799E-2</v>
+        <v>8.4973136369636392E-3</v>
       </c>
       <c r="N25" s="2">
-        <v>2.1333935376342001E-2</v>
+        <v>8.51639700905997E-3</v>
       </c>
       <c r="O25" s="2">
-        <v>2.1349906495591601E-2</v>
+        <v>8.5319225462757893E-3</v>
       </c>
       <c r="P25" s="2">
-        <v>2.13586909096301E-2</v>
+        <v>8.5367745788500898E-3</v>
       </c>
       <c r="Q25" s="2">
-        <v>2.13586909096301E-2</v>
+        <v>8.5503588195252195E-3</v>
       </c>
       <c r="R25" s="2">
-        <v>2.1364279906013799E-2</v>
+        <v>8.56103232416674E-3</v>
       </c>
       <c r="S25" s="2">
-        <v>2.1367475323668599E-2</v>
+        <v>8.5865842671771896E-3</v>
       </c>
       <c r="T25" s="2">
-        <v>2.1389819371155E-2</v>
+        <v>8.5901421020576994E-3</v>
       </c>
       <c r="U25" s="2">
-        <v>2.1412995102688501E-2</v>
+        <v>8.6056676392735204E-3</v>
       </c>
       <c r="V25" s="2">
-        <v>2.1405006558551501E-2</v>
+        <v>8.6182824404557306E-3</v>
       </c>
       <c r="W25" s="23" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A26" s="17" t="s">
         <v>44</v>
       </c>
       <c r="B26" s="2">
-        <f>$I$12*B22*(1-$B$16)*$I$14</f>
-        <v>6.2343240623357297E-2</v>
+        <f t="shared" ref="B26:V26" si="5">$I$12*B22*(1-$B$16)*$I$14</f>
+        <v>0.10721074516785122</v>
       </c>
       <c r="C26" s="2">
-        <f>$I$12*C22*(1-$B$16)*$I$14</f>
-        <v>3.6932026107468922E-2</v>
+        <f t="shared" si="5"/>
+        <v>7.9060795893335006E-2</v>
       </c>
       <c r="D26" s="2">
-        <f>$I$12*D22*(1-$B$16)*$I$14</f>
-        <v>2.6321915662421595E-2</v>
+        <f t="shared" si="5"/>
+        <v>5.340201213372886E-2</v>
       </c>
       <c r="E26" s="2">
-        <f>$I$12*E22*(1-$B$16)*$I$14</f>
-        <v>1.6295361291851863E-2</v>
+        <f t="shared" si="5"/>
+        <v>4.925743774113224E-2</v>
       </c>
       <c r="F26" s="2">
-        <f>$I$12*F22*(1-$B$16)*$I$14</f>
-        <v>9.3103719155290341E-3</v>
+        <f t="shared" si="5"/>
+        <v>2.7212722851870357E-2</v>
       </c>
       <c r="G26" s="2">
-        <f>$I$12*G22*(1-$B$16)*$I$14</f>
-        <v>4.2528859367231388E-3</v>
+        <f t="shared" si="5"/>
+        <v>1.8680425702311463E-2</v>
       </c>
       <c r="H26" s="2">
-        <f>$I$12*H22*(1-$B$16)*$I$14</f>
-        <v>3.9787914168927497E-4</v>
+        <f t="shared" si="5"/>
+        <v>1.2438144057141946E-2</v>
       </c>
       <c r="I26" s="2">
-        <f>$I$12*I22*(1-$B$16)*$I$14</f>
-        <v>-2.5729517829239782E-3</v>
+        <f t="shared" si="5"/>
+        <v>8.843969143882165E-3</v>
       </c>
       <c r="J26" s="2">
-        <f>$I$12*J22*(1-$B$16)*$I$14</f>
-        <v>-4.88949256342598E-3</v>
+        <f t="shared" si="5"/>
+        <v>3.8306919585972977E-3</v>
       </c>
       <c r="K26" s="2">
-        <f>$I$12*K22*(1-$B$16)*$I$14</f>
-        <v>-6.7639454087176755E-3</v>
+        <f t="shared" si="5"/>
+        <v>7.8470608499829229E-4</v>
       </c>
       <c r="L26" s="2">
-        <f>$I$12*L22*(1-$B$16)*$I$14</f>
-        <v>-8.2935696645453326E-3</v>
+        <f t="shared" si="5"/>
+        <v>-1.6931967918554704E-3</v>
       </c>
       <c r="M26" s="2">
-        <f>$I$12*M22*(1-$B$16)*$I$14</f>
-        <v>-9.549099400542601E-3</v>
+        <f t="shared" si="5"/>
+        <v>-3.7223804144707728E-3</v>
       </c>
       <c r="N26" s="2">
-        <f>$I$12*N22*(1-$B$16)*$I$14</f>
-        <v>-1.060126868634313E-2</v>
+        <f t="shared" si="5"/>
+        <v>-5.4443129221149128E-3</v>
       </c>
       <c r="O26" s="2">
-        <f>$I$12*O22*(1-$B$16)*$I$14</f>
-        <v>-1.148544455676374E-2</v>
+        <f t="shared" si="5"/>
+        <v>-6.8855195909005105E-3</v>
       </c>
       <c r="P26" s="2">
-        <f>$I$12*P22*(1-$B$16)*$I$14</f>
-        <v>-1.2236994046621257E-2</v>
+        <f t="shared" si="5"/>
+        <v>-8.1101031714330557E-3</v>
       </c>
       <c r="Q26" s="2">
-        <f>$I$12*Q22*(1-$B$16)*$I$14</f>
-        <v>-1.2873600673324097E-2</v>
+        <f t="shared" si="5"/>
+        <v>-9.168903776261738E-3</v>
       </c>
       <c r="R26" s="2">
-        <f>$I$12*R22*(1-$B$16)*$I$14</f>
-        <v>-1.3439473230393288E-2</v>
+        <f t="shared" si="5"/>
+        <v>-1.0081815362471018E-2</v>
       </c>
       <c r="S26" s="2">
-        <f>$I$12*S22*(1-$B$16)*$I$14</f>
-        <v>-1.3925769959124626E-2</v>
+        <f t="shared" si="5"/>
+        <v>-1.0873152766497465E-2</v>
       </c>
       <c r="T26" s="2">
-        <f>$I$12*T22*(1-$B$16)*$I$14</f>
-        <v>-1.4341332618222312E-2</v>
+        <f t="shared" si="5"/>
+        <v>-1.1562809945425542E-2</v>
       </c>
       <c r="U26" s="2">
-        <f>$I$12*U22*(1-$B$16)*$I$14</f>
-        <v>-1.4703844725094766E-2</v>
+        <f t="shared" si="5"/>
+        <v>-1.2170680856339712E-2</v>
       </c>
       <c r="V26" s="2">
-        <f>$I$12*V22*(1-$B$16)*$I$14</f>
-        <v>-1.5039831555854595E-2</v>
+        <f t="shared" si="5"/>
+        <v>-1.2712238576972339E-2</v>
       </c>
       <c r="W26" s="23" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A27" s="19" t="s">
         <v>53</v>
       </c>
       <c r="B27" s="21">
         <f>((1+$L$11)*(B26^2))/(PI()*$I$17)</f>
-        <v>3.0778339722596973E-4</v>
+        <v>9.102130786945075E-4</v>
       </c>
       <c r="C27" s="21">
         <f>((1+$L$11)*(C26^2))/(PI()*$I$17)</f>
-        <v>1.0801217468867552E-4</v>
+        <v>4.949813164342304E-4</v>
       </c>
       <c r="D27" s="21">
-        <f t="shared" ref="D27:V27" si="3">((1+$L$11)*(D26^2))/(PI()*$I$17)</f>
-        <v>5.4865763724146713E-5</v>
+        <f t="shared" ref="D27:V27" si="6">((1+$L$11)*(D26^2))/(PI()*$I$17)</f>
+        <v>2.2583002602321459E-4</v>
       </c>
       <c r="E27" s="21">
-        <f t="shared" si="3"/>
-        <v>2.1027828680488288E-5</v>
+        <f t="shared" si="6"/>
+        <v>1.9213658905250746E-4</v>
       </c>
       <c r="F27" s="21">
-        <f t="shared" si="3"/>
-        <v>6.8643671134060467E-6</v>
+        <f t="shared" si="6"/>
+        <v>5.8642224952432596E-5</v>
       </c>
       <c r="G27" s="21">
-        <f t="shared" si="3"/>
-        <v>1.4322997375785515E-6</v>
+        <f t="shared" si="6"/>
+        <v>2.7633759933155704E-5</v>
       </c>
       <c r="H27" s="21">
-        <f t="shared" si="3"/>
-        <v>1.2536282988907236E-8</v>
+        <f t="shared" si="6"/>
+        <v>1.2251171156119612E-5</v>
       </c>
       <c r="I27" s="21">
-        <f t="shared" si="3"/>
-        <v>5.2423949618945873E-7</v>
+        <f t="shared" si="6"/>
+        <v>6.1938527969972284E-6</v>
       </c>
       <c r="J27" s="21">
-        <f t="shared" si="3"/>
-        <v>1.8931892170640665E-6</v>
+        <f t="shared" si="6"/>
+        <v>1.162039530909637E-6</v>
       </c>
       <c r="K27" s="21">
-        <f t="shared" si="3"/>
-        <v>3.622985783794193E-6</v>
+        <f t="shared" si="6"/>
+        <v>4.8761884681389963E-8</v>
       </c>
       <c r="L27" s="21">
-        <f t="shared" si="3"/>
-        <v>5.4469004296751116E-6</v>
+        <f t="shared" si="6"/>
+        <v>2.2702898955059437E-7</v>
       </c>
       <c r="M27" s="21">
-        <f t="shared" si="3"/>
-        <v>7.2208990016105725E-6</v>
+        <f t="shared" si="6"/>
+        <v>1.0972559670305719E-6</v>
       </c>
       <c r="N27" s="21">
-        <f t="shared" si="3"/>
-        <v>8.8998384993264422E-6</v>
+        <f t="shared" si="6"/>
+        <v>2.3472135339238957E-6</v>
       </c>
       <c r="O27" s="21">
-        <f t="shared" si="3"/>
-        <v>1.0446289605809911E-5</v>
+        <f t="shared" si="6"/>
+        <v>3.7543942748468985E-6</v>
       </c>
       <c r="P27" s="21">
-        <f t="shared" si="3"/>
-        <v>1.1858122700642124E-5</v>
+        <f t="shared" si="6"/>
+        <v>5.2085783385320108E-6</v>
       </c>
       <c r="Q27" s="21">
-        <f t="shared" si="3"/>
-        <v>1.3124008698455337E-5</v>
+        <f t="shared" si="6"/>
+        <v>6.6573481982707112E-6</v>
       </c>
       <c r="R27" s="21">
-        <f t="shared" si="3"/>
-        <v>1.4303125045714213E-5</v>
+        <f t="shared" si="6"/>
+        <v>8.049036956644549E-6</v>
       </c>
       <c r="S27" s="21">
-        <f t="shared" si="3"/>
-        <v>1.535694666141137E-5</v>
+        <f t="shared" si="6"/>
+        <v>9.362189384393714E-6</v>
       </c>
       <c r="T27" s="21">
-        <f t="shared" si="3"/>
-        <v>1.6287163622216411E-5</v>
+        <f t="shared" si="6"/>
+        <v>1.0587494969865056E-5</v>
       </c>
       <c r="U27" s="21">
-        <f t="shared" si="3"/>
-        <v>1.712096573301196E-5</v>
+        <f t="shared" si="6"/>
+        <v>1.1729950814749983E-5</v>
       </c>
       <c r="V27" s="21">
-        <f t="shared" si="3"/>
-        <v>1.7912342585870219E-5</v>
+        <f t="shared" si="6"/>
+        <v>1.2797069015783988E-5</v>
       </c>
       <c r="W27" s="23" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A28" s="19" t="s">
         <v>21</v>
       </c>
@@ -1857,7 +1850,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A29" s="19" t="s">
         <v>20</v>
       </c>
@@ -1928,7 +1921,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A30" s="24"/>
       <c r="W30" s="22"/>
     </row>

</xml_diff>

<commit_message>
@arnoldgreg98 Fixed the Excel Sheet, no change in matlab
p.s. Pushed by Eddie
</commit_message>
<xml_diff>
--- a/Wing Tail Drag Buildup/Drag.xlsx
+++ b/Wing Tail Drag Buildup/Drag.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e\Documents\GitHub\Senior-Design\Wing Tail Drag Buildup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eddie.hsieh\Documents\GitHub\Wing Tail Drag Buildup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E7596C-D420-4842-B20A-2BE0440FC25E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C17981-5778-4C31-9DA3-E7AAE0ED40B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="2010" windowWidth="24525" windowHeight="17850" xr2:uid="{82617F0D-A785-403D-9CC0-085A46D2A0AD}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{82617F0D-A785-403D-9CC0-085A46D2A0AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1149,6 +1149,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-C32E-4DA3-8E3E-CA1FA66392AB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1164,6 +1169,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-C32E-4DA3-8E3E-CA1FA66392AB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1179,6 +1189,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-C32E-4DA3-8E3E-CA1FA66392AB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -1548,7 +1563,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>(Sheet1!$A$26,Sheet1!$A$30,Sheet1!$A$32,Sheet1!$A$38,Sheet1!$A$41,Sheet1!$A$42,Sheet1!$A$43,Sheet1!$A$50,Sheet1!$A$52)</c:f>
+              <c:f>(Sheet1!$A$55,Sheet1!$A$56,Sheet1!$A$29,Sheet1!$A$38,Sheet1!$A$41,Sheet1!$A$42,Sheet1!$A$43,Sheet1!$A$50,Sheet1!$A$52)</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -1583,7 +1598,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$H$26,Sheet1!$H$30,Sheet1!$H$32,Sheet1!$H$38,Sheet1!$H$41,Sheet1!$H$42,Sheet1!$H$43,Sheet1!$H$50,Sheet1!$H$52)</c:f>
+              <c:f>(Sheet1!$H$55,Sheet1!$H$56,Sheet1!$H$29,Sheet1!$H$38,Sheet1!$H$41,Sheet1!$H$42,Sheet1!$H$43,Sheet1!$H$50,Sheet1!$H$52)</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -3175,10 +3190,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470D6C11-8322-4BAC-B928-8395D64AAF23}">
-  <dimension ref="A1:W54"/>
+  <dimension ref="A1:W56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AI46" sqref="AI46"/>
+    <sheetView tabSelected="1" topLeftCell="D17" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4046,181 +4061,184 @@
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
-        <v>78</v>
+      <c r="A26" s="26" t="s">
+        <v>43</v>
       </c>
       <c r="B26" s="2">
-        <f>SUM(B24:B25)</f>
-        <v>7.5956033152108748E-2</v>
+        <f>$I$12*B22*(1-$B$16)*$I$14</f>
+        <v>0.10721074516785122</v>
       </c>
       <c r="C26" s="2">
-        <f t="shared" ref="C26:V26" si="5">SUM(C24:C25)</f>
-        <v>5.0533256419405093E-2</v>
+        <f>$I$12*C22*(1-$B$16)*$I$14</f>
+        <v>7.9060795893335006E-2</v>
       </c>
       <c r="D26" s="2">
-        <f t="shared" si="5"/>
-        <v>3.1545182759264739E-2</v>
+        <f>$I$12*D22*(1-$B$16)*$I$14</f>
+        <v>5.340201213372886E-2</v>
       </c>
       <c r="E26" s="2">
-        <f t="shared" si="5"/>
-        <v>2.1487520413685623E-2</v>
+        <f>$I$12*E22*(1-$B$16)*$I$14</f>
+        <v>4.925743774113224E-2</v>
       </c>
       <c r="F26" s="2">
-        <f t="shared" si="5"/>
-        <v>1.5836024451445274E-2</v>
+        <f>$I$12*F22*(1-$B$16)*$I$14</f>
+        <v>2.7212722851870357E-2</v>
       </c>
       <c r="G26" s="2">
-        <f t="shared" si="5"/>
-        <v>1.3206980896168783E-2</v>
+        <f>$I$12*G22*(1-$B$16)*$I$14</f>
+        <v>1.8680425702311463E-2</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" si="5"/>
-        <v>1.1731214972786497E-2</v>
+        <f>$I$12*H22*(1-$B$16)*$I$14</f>
+        <v>1.2438144057141946E-2</v>
       </c>
       <c r="I26" s="2">
-        <f t="shared" si="5"/>
-        <v>1.0879538691473404E-2</v>
+        <f>$I$12*I22*(1-$B$16)*$I$14</f>
+        <v>8.843969143882165E-3</v>
       </c>
       <c r="J26" s="2">
-        <f t="shared" si="5"/>
-        <v>1.0359368847452102E-2</v>
+        <f>$I$12*J22*(1-$B$16)*$I$14</f>
+        <v>3.8306919585972977E-3</v>
       </c>
       <c r="K26" s="2">
-        <f t="shared" si="5"/>
-        <v>9.9480185112243227E-3</v>
+        <f>$I$12*K22*(1-$B$16)*$I$14</f>
+        <v>7.8470608499829229E-4</v>
       </c>
       <c r="L26" s="2">
-        <f t="shared" si="5"/>
-        <v>9.6461172407927252E-3</v>
+        <f>$I$12*L22*(1-$B$16)*$I$14</f>
+        <v>-1.6931967918554704E-3</v>
       </c>
       <c r="M26" s="2">
-        <f t="shared" si="5"/>
-        <v>9.4144742796864987E-3</v>
+        <f>$I$12*M22*(1-$B$16)*$I$14</f>
+        <v>-3.7223804144707728E-3</v>
       </c>
       <c r="N26" s="2">
-        <f t="shared" si="5"/>
-        <v>9.2461083148904066E-3</v>
+        <f>$I$12*N22*(1-$B$16)*$I$14</f>
+        <v>-5.4443129221149128E-3</v>
       </c>
       <c r="O26" s="2">
-        <f t="shared" si="5"/>
-        <v>9.1197186347101618E-3</v>
+        <f>$I$12*O22*(1-$B$16)*$I$14</f>
+        <v>-6.8855195909005105E-3</v>
       </c>
       <c r="P26" s="2">
-        <f t="shared" si="5"/>
-        <v>9.0155381666054395E-3</v>
+        <f>$I$12*P22*(1-$B$16)*$I$14</f>
+        <v>-8.1101031714330557E-3</v>
       </c>
       <c r="Q26" s="2">
-        <f t="shared" si="5"/>
-        <v>8.9442388080117861E-3</v>
+        <f>$I$12*Q22*(1-$B$16)*$I$14</f>
+        <v>-9.168903776261738E-3</v>
       </c>
       <c r="R26" s="2">
-        <f t="shared" si="5"/>
-        <v>8.8880342965425001E-3</v>
+        <f>$I$12*R22*(1-$B$16)*$I$14</f>
+        <v>-1.0081815362471018E-2</v>
       </c>
       <c r="S26" s="2">
-        <f t="shared" si="5"/>
-        <v>8.8603189023480754E-3</v>
+        <f>$I$12*S22*(1-$B$16)*$I$14</f>
+        <v>-1.0873152766497465E-2</v>
       </c>
       <c r="T26" s="2">
-        <f t="shared" si="5"/>
-        <v>8.8210273199181115E-3</v>
+        <f>$I$12*T22*(1-$B$16)*$I$14</f>
+        <v>-1.1562809945425542E-2</v>
       </c>
       <c r="U26" s="2">
-        <f t="shared" si="5"/>
-        <v>8.8017692048181113E-3</v>
+        <f>$I$12*U22*(1-$B$16)*$I$14</f>
+        <v>-1.2170680856339712E-2</v>
       </c>
       <c r="V26" s="2">
-        <f t="shared" si="5"/>
-        <v>8.7859108805507374E-3</v>
+        <f>$I$12*V22*(1-$B$16)*$I$14</f>
+        <v>-1.2712238576972339E-2</v>
+      </c>
+      <c r="W26" s="21" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="2">
-        <f>$I$12*B22*(1-$B$16)*$I$14</f>
-        <v>0.10721074516785122</v>
-      </c>
-      <c r="C27" s="2">
-        <f>$I$12*C22*(1-$B$16)*$I$14</f>
-        <v>7.9060795893335006E-2</v>
-      </c>
-      <c r="D27" s="2">
-        <f>$I$12*D22*(1-$B$16)*$I$14</f>
-        <v>5.340201213372886E-2</v>
-      </c>
-      <c r="E27" s="2">
-        <f>$I$12*E22*(1-$B$16)*$I$14</f>
-        <v>4.925743774113224E-2</v>
-      </c>
-      <c r="F27" s="2">
-        <f>$I$12*F22*(1-$B$16)*$I$14</f>
-        <v>2.7212722851870357E-2</v>
-      </c>
-      <c r="G27" s="2">
-        <f>$I$12*G22*(1-$B$16)*$I$14</f>
-        <v>1.8680425702311463E-2</v>
-      </c>
-      <c r="H27" s="2">
-        <f>$I$12*H22*(1-$B$16)*$I$14</f>
-        <v>1.2438144057141946E-2</v>
-      </c>
-      <c r="I27" s="2">
-        <f>$I$12*I22*(1-$B$16)*$I$14</f>
-        <v>8.843969143882165E-3</v>
-      </c>
-      <c r="J27" s="2">
-        <f>$I$12*J22*(1-$B$16)*$I$14</f>
-        <v>3.8306919585972977E-3</v>
-      </c>
-      <c r="K27" s="2">
-        <f>$I$12*K22*(1-$B$16)*$I$14</f>
-        <v>7.8470608499829229E-4</v>
-      </c>
-      <c r="L27" s="2">
-        <f>$I$12*L22*(1-$B$16)*$I$14</f>
-        <v>-1.6931967918554704E-3</v>
-      </c>
-      <c r="M27" s="2">
-        <f>$I$12*M22*(1-$B$16)*$I$14</f>
-        <v>-3.7223804144707728E-3</v>
-      </c>
-      <c r="N27" s="2">
-        <f>$I$12*N22*(1-$B$16)*$I$14</f>
-        <v>-5.4443129221149128E-3</v>
-      </c>
-      <c r="O27" s="2">
-        <f>$I$12*O22*(1-$B$16)*$I$14</f>
-        <v>-6.8855195909005105E-3</v>
-      </c>
-      <c r="P27" s="2">
-        <f>$I$12*P22*(1-$B$16)*$I$14</f>
-        <v>-8.1101031714330557E-3</v>
-      </c>
-      <c r="Q27" s="2">
-        <f>$I$12*Q22*(1-$B$16)*$I$14</f>
-        <v>-9.168903776261738E-3</v>
-      </c>
-      <c r="R27" s="2">
-        <f>$I$12*R22*(1-$B$16)*$I$14</f>
-        <v>-1.0081815362471018E-2</v>
-      </c>
-      <c r="S27" s="2">
-        <f>$I$12*S22*(1-$B$16)*$I$14</f>
-        <v>-1.0873152766497465E-2</v>
-      </c>
-      <c r="T27" s="2">
-        <f>$I$12*T22*(1-$B$16)*$I$14</f>
-        <v>-1.1562809945425542E-2</v>
-      </c>
-      <c r="U27" s="2">
-        <f>$I$12*U22*(1-$B$16)*$I$14</f>
-        <v>-1.2170680856339712E-2</v>
-      </c>
-      <c r="V27" s="2">
-        <f>$I$12*V22*(1-$B$16)*$I$14</f>
-        <v>-1.2712238576972339E-2</v>
+      <c r="A27" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="19">
+        <f>((1+$L$11)*(B26^2))/(PI()*$I$17)</f>
+        <v>9.102130786945075E-4</v>
+      </c>
+      <c r="C27" s="19">
+        <f>((1+$L$11)*(C26^2))/(PI()*$I$17)</f>
+        <v>4.949813164342304E-4</v>
+      </c>
+      <c r="D27" s="19">
+        <f t="shared" ref="D27:V27" si="5">((1+$L$11)*(D26^2))/(PI()*$I$17)</f>
+        <v>2.2583002602321459E-4</v>
+      </c>
+      <c r="E27" s="19">
+        <f t="shared" si="5"/>
+        <v>1.9213658905250746E-4</v>
+      </c>
+      <c r="F27" s="19">
+        <f t="shared" si="5"/>
+        <v>5.8642224952432596E-5</v>
+      </c>
+      <c r="G27" s="19">
+        <f t="shared" si="5"/>
+        <v>2.7633759933155704E-5</v>
+      </c>
+      <c r="H27" s="19">
+        <f t="shared" si="5"/>
+        <v>1.2251171156119612E-5</v>
+      </c>
+      <c r="I27" s="19">
+        <f t="shared" si="5"/>
+        <v>6.1938527969972284E-6</v>
+      </c>
+      <c r="J27" s="19">
+        <f t="shared" si="5"/>
+        <v>1.162039530909637E-6</v>
+      </c>
+      <c r="K27" s="19">
+        <f t="shared" si="5"/>
+        <v>4.8761884681389963E-8</v>
+      </c>
+      <c r="L27" s="19">
+        <f t="shared" si="5"/>
+        <v>2.2702898955059437E-7</v>
+      </c>
+      <c r="M27" s="19">
+        <f t="shared" si="5"/>
+        <v>1.0972559670305719E-6</v>
+      </c>
+      <c r="N27" s="19">
+        <f t="shared" si="5"/>
+        <v>2.3472135339238957E-6</v>
+      </c>
+      <c r="O27" s="19">
+        <f t="shared" si="5"/>
+        <v>3.7543942748468985E-6</v>
+      </c>
+      <c r="P27" s="19">
+        <f t="shared" si="5"/>
+        <v>5.2085783385320108E-6</v>
+      </c>
+      <c r="Q27" s="19">
+        <f t="shared" si="5"/>
+        <v>6.6573481982707112E-6</v>
+      </c>
+      <c r="R27" s="19">
+        <f t="shared" si="5"/>
+        <v>8.049036956644549E-6</v>
+      </c>
+      <c r="S27" s="19">
+        <f t="shared" si="5"/>
+        <v>9.362189384393714E-6</v>
+      </c>
+      <c r="T27" s="19">
+        <f t="shared" si="5"/>
+        <v>1.0587494969865056E-5</v>
+      </c>
+      <c r="U27" s="19">
+        <f t="shared" si="5"/>
+        <v>1.1729950814749983E-5</v>
+      </c>
+      <c r="V27" s="19">
+        <f t="shared" si="5"/>
+        <v>1.2797069015783988E-5</v>
       </c>
       <c r="W27" s="21" t="s">
         <v>61</v>
@@ -4228,324 +4246,143 @@
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" s="19">
-        <f>((1+$L$11)*(B27^2))/(PI()*$I$17)</f>
-        <v>9.102130786945075E-4</v>
-      </c>
-      <c r="C28" s="19">
-        <f>((1+$L$11)*(C27^2))/(PI()*$I$17)</f>
-        <v>4.949813164342304E-4</v>
-      </c>
-      <c r="D28" s="19">
-        <f t="shared" ref="D28:V28" si="6">((1+$L$11)*(D27^2))/(PI()*$I$17)</f>
-        <v>2.2583002602321459E-4</v>
-      </c>
-      <c r="E28" s="19">
-        <f t="shared" si="6"/>
-        <v>1.9213658905250746E-4</v>
-      </c>
-      <c r="F28" s="19">
-        <f t="shared" si="6"/>
-        <v>5.8642224952432596E-5</v>
-      </c>
-      <c r="G28" s="19">
-        <f t="shared" si="6"/>
-        <v>2.7633759933155704E-5</v>
-      </c>
-      <c r="H28" s="19">
-        <f t="shared" si="6"/>
-        <v>1.2251171156119612E-5</v>
-      </c>
-      <c r="I28" s="19">
-        <f t="shared" si="6"/>
-        <v>6.1938527969972284E-6</v>
-      </c>
-      <c r="J28" s="19">
-        <f t="shared" si="6"/>
-        <v>1.162039530909637E-6</v>
-      </c>
-      <c r="K28" s="19">
-        <f t="shared" si="6"/>
-        <v>4.8761884681389963E-8</v>
-      </c>
-      <c r="L28" s="19">
-        <f t="shared" si="6"/>
-        <v>2.2702898955059437E-7</v>
-      </c>
-      <c r="M28" s="19">
-        <f t="shared" si="6"/>
-        <v>1.0972559670305719E-6</v>
-      </c>
-      <c r="N28" s="19">
-        <f t="shared" si="6"/>
-        <v>2.3472135339238957E-6</v>
-      </c>
-      <c r="O28" s="19">
-        <f t="shared" si="6"/>
-        <v>3.7543942748468985E-6</v>
-      </c>
-      <c r="P28" s="19">
-        <f t="shared" si="6"/>
-        <v>5.2085783385320108E-6</v>
-      </c>
-      <c r="Q28" s="19">
-        <f t="shared" si="6"/>
-        <v>6.6573481982707112E-6</v>
-      </c>
-      <c r="R28" s="19">
-        <f t="shared" si="6"/>
-        <v>8.049036956644549E-6</v>
-      </c>
-      <c r="S28" s="19">
-        <f t="shared" si="6"/>
-        <v>9.362189384393714E-6</v>
-      </c>
-      <c r="T28" s="19">
-        <f t="shared" si="6"/>
-        <v>1.0587494969865056E-5</v>
-      </c>
-      <c r="U28" s="19">
-        <f t="shared" si="6"/>
-        <v>1.1729950814749983E-5</v>
-      </c>
-      <c r="V28" s="19">
-        <f t="shared" si="6"/>
-        <v>1.2797069015783988E-5</v>
+        <v>20</v>
+      </c>
+      <c r="B28" s="2">
+        <v>3.0822223606353201E-3</v>
+      </c>
+      <c r="C28" s="2">
+        <v>2.3200506591923601E-3</v>
+      </c>
+      <c r="D28" s="2">
+        <v>2E-3</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1.7926278417938299E-3</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1.7103132980379901E-3</v>
+      </c>
+      <c r="G28" s="2">
+        <v>1.67982642998028E-3</v>
+      </c>
+      <c r="H28" s="2">
+        <v>1.66458299595142E-3</v>
+      </c>
+      <c r="I28" s="2">
+        <v>1.6554369355341E-3</v>
+      </c>
+      <c r="J28" s="2">
+        <v>1.6523882487283299E-3</v>
+      </c>
+      <c r="K28" s="2">
+        <v>1.6523882487283299E-3</v>
+      </c>
+      <c r="L28" s="2">
+        <v>1.6554369355341E-3</v>
+      </c>
+      <c r="M28" s="2">
+        <v>1.6554369355341E-3</v>
+      </c>
+      <c r="N28" s="2">
+        <v>1.6554369355341E-3</v>
+      </c>
+      <c r="O28" s="2">
+        <v>1.6615343091456499E-3</v>
+      </c>
+      <c r="P28" s="2">
+        <v>1.66458299595142E-3</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>1.6676316827571899E-3</v>
+      </c>
+      <c r="R28" s="2">
+        <v>1.6737290563687301E-3</v>
+      </c>
+      <c r="S28" s="2">
+        <v>1.6767777431745E-3</v>
+      </c>
+      <c r="T28" s="2">
+        <v>1.67982642998028E-3</v>
+      </c>
+      <c r="U28" s="2">
+        <v>1.6889724903975899E-3</v>
+      </c>
+      <c r="V28" s="2">
+        <v>1.6889724903975899E-3</v>
       </c>
       <c r="W28" s="21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A29" s="23" t="s">
-        <v>20</v>
+      <c r="A29" s="28" t="s">
+        <v>79</v>
       </c>
       <c r="B29" s="2">
-        <v>3.0822223606353201E-3</v>
+        <v>1.71032388663968E-3</v>
       </c>
       <c r="C29" s="2">
-        <v>2.3200506591923601E-3</v>
+        <v>1.6829933561714899E-3</v>
       </c>
       <c r="D29" s="2">
-        <v>2E-3</v>
+        <v>1.66646942800789E-3</v>
       </c>
       <c r="E29" s="2">
-        <v>1.7926278417938299E-3</v>
+        <v>1.65707204401536E-3</v>
       </c>
       <c r="F29" s="2">
-        <v>1.7103132980379901E-3</v>
+        <v>1.6508071213536799E-3</v>
       </c>
       <c r="G29" s="2">
-        <v>1.67982642998028E-3</v>
+        <v>1.6445421986920001E-3</v>
       </c>
       <c r="H29" s="2">
-        <v>1.66458299595142E-3</v>
+        <v>1.64054811585176E-3</v>
       </c>
       <c r="I29" s="2">
-        <v>1.6554369355341E-3</v>
+        <v>1.63514481469947E-3</v>
       </c>
       <c r="J29" s="2">
-        <v>1.6523882487283299E-3</v>
+        <v>1.63514481469947E-3</v>
       </c>
       <c r="K29" s="2">
-        <v>1.6523882487283299E-3</v>
+        <v>1.63827727603031E-3</v>
       </c>
       <c r="L29" s="2">
-        <v>1.6554369355341E-3</v>
+        <v>1.63514481469947E-3</v>
       </c>
       <c r="M29" s="2">
-        <v>1.6554369355341E-3</v>
+        <v>1.63514481469947E-3</v>
       </c>
       <c r="N29" s="2">
-        <v>1.6554369355341E-3</v>
+        <v>1.6414097373611499E-3</v>
       </c>
       <c r="O29" s="2">
-        <v>1.6615343091456499E-3</v>
+        <v>1.63827727603031E-3</v>
       </c>
       <c r="P29" s="2">
-        <v>1.66458299595142E-3</v>
+        <v>1.6422713588705501E-3</v>
       </c>
       <c r="Q29" s="2">
-        <v>1.6676316827571899E-3</v>
+        <v>1.6414097373611499E-3</v>
       </c>
       <c r="R29" s="2">
-        <v>1.6737290563687301E-3</v>
+        <v>1.64767466002284E-3</v>
       </c>
       <c r="S29" s="2">
-        <v>1.6767777431745E-3</v>
+        <v>1.6445421986920001E-3</v>
       </c>
       <c r="T29" s="2">
-        <v>1.67982642998028E-3</v>
+        <v>1.6539395826845201E-3</v>
       </c>
       <c r="U29" s="2">
-        <v>1.6889724903975899E-3</v>
+        <v>1.6508071213536799E-3</v>
       </c>
       <c r="V29" s="2">
-        <v>1.6889724903975899E-3</v>
+        <v>1.66020450534621E-3</v>
       </c>
       <c r="W29" s="21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="B30" s="2">
-        <f>SUM(B28:B29)</f>
-        <v>3.9924354393298276E-3</v>
-      </c>
-      <c r="C30" s="2">
-        <f t="shared" ref="C30:V30" si="7">SUM(C28:C29)</f>
-        <v>2.8150319756265908E-3</v>
-      </c>
-      <c r="D30" s="2">
-        <f t="shared" si="7"/>
-        <v>2.2258300260232147E-3</v>
-      </c>
-      <c r="E30" s="2">
-        <f t="shared" si="7"/>
-        <v>1.9847644308463373E-3</v>
-      </c>
-      <c r="F30" s="2">
-        <f t="shared" si="7"/>
-        <v>1.7689555229904227E-3</v>
-      </c>
-      <c r="G30" s="2">
-        <f t="shared" si="7"/>
-        <v>1.7074601899134357E-3</v>
-      </c>
-      <c r="H30" s="2">
-        <f t="shared" si="7"/>
-        <v>1.6768341671075397E-3</v>
-      </c>
-      <c r="I30" s="2">
-        <f t="shared" si="7"/>
-        <v>1.6616307883310971E-3</v>
-      </c>
-      <c r="J30" s="2">
-        <f t="shared" si="7"/>
-        <v>1.6535502882592396E-3</v>
-      </c>
-      <c r="K30" s="2">
-        <f t="shared" si="7"/>
-        <v>1.6524370106130112E-3</v>
-      </c>
-      <c r="L30" s="2">
-        <f t="shared" si="7"/>
-        <v>1.6556639645236505E-3</v>
-      </c>
-      <c r="M30" s="2">
-        <f t="shared" si="7"/>
-        <v>1.6565341915011306E-3</v>
-      </c>
-      <c r="N30" s="2">
-        <f t="shared" si="7"/>
-        <v>1.6577841490680238E-3</v>
-      </c>
-      <c r="O30" s="2">
-        <f t="shared" si="7"/>
-        <v>1.6652887034204968E-3</v>
-      </c>
-      <c r="P30" s="2">
-        <f t="shared" si="7"/>
-        <v>1.6697915742899521E-3</v>
-      </c>
-      <c r="Q30" s="2">
-        <f t="shared" si="7"/>
-        <v>1.6742890309554607E-3</v>
-      </c>
-      <c r="R30" s="2">
-        <f t="shared" si="7"/>
-        <v>1.6817780933253746E-3</v>
-      </c>
-      <c r="S30" s="2">
-        <f t="shared" si="7"/>
-        <v>1.6861399325588937E-3</v>
-      </c>
-      <c r="T30" s="2">
-        <f t="shared" si="7"/>
-        <v>1.6904139249501451E-3</v>
-      </c>
-      <c r="U30" s="2">
-        <f t="shared" si="7"/>
-        <v>1.7007024412123398E-3</v>
-      </c>
-      <c r="V30" s="2">
-        <f t="shared" si="7"/>
-        <v>1.7017695594133738E-3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A32" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="B32" s="2">
-        <v>1.71032388663968E-3</v>
-      </c>
-      <c r="C32" s="2">
-        <v>1.6829933561714899E-3</v>
-      </c>
-      <c r="D32" s="2">
-        <v>1.66646942800789E-3</v>
-      </c>
-      <c r="E32" s="2">
-        <v>1.65707204401536E-3</v>
-      </c>
-      <c r="F32" s="2">
-        <v>1.6508071213536799E-3</v>
-      </c>
-      <c r="G32" s="2">
-        <v>1.6445421986920001E-3</v>
-      </c>
-      <c r="H32" s="2">
-        <v>1.64054811585176E-3</v>
-      </c>
-      <c r="I32" s="2">
-        <v>1.63514481469947E-3</v>
-      </c>
-      <c r="J32" s="2">
-        <v>1.63514481469947E-3</v>
-      </c>
-      <c r="K32" s="2">
-        <v>1.63827727603031E-3</v>
-      </c>
-      <c r="L32" s="2">
-        <v>1.63514481469947E-3</v>
-      </c>
-      <c r="M32" s="2">
-        <v>1.63514481469947E-3</v>
-      </c>
-      <c r="N32" s="2">
-        <v>1.6414097373611499E-3</v>
-      </c>
-      <c r="O32" s="2">
-        <v>1.63827727603031E-3</v>
-      </c>
-      <c r="P32" s="2">
-        <v>1.6422713588705501E-3</v>
-      </c>
-      <c r="Q32" s="2">
-        <v>1.6414097373611499E-3</v>
-      </c>
-      <c r="R32" s="2">
-        <v>1.64767466002284E-3</v>
-      </c>
-      <c r="S32" s="2">
-        <v>1.6445421986920001E-3</v>
-      </c>
-      <c r="T32" s="2">
-        <v>1.6539395826845201E-3</v>
-      </c>
-      <c r="U32" s="2">
-        <v>1.6508071213536799E-3</v>
-      </c>
-      <c r="V32" s="2">
-        <v>1.66020450534621E-3</v>
-      </c>
-      <c r="W32" s="21" t="s">
         <v>59</v>
       </c>
     </row>
@@ -4771,83 +4608,83 @@
         <v>2.5943952966763138E-2</v>
       </c>
       <c r="C38" s="2">
-        <f t="shared" ref="C38:V38" si="8">SUM(C36:C37)</f>
+        <f t="shared" ref="C38:V38" si="6">SUM(C36:C37)</f>
         <v>1.54636722038725E-2</v>
       </c>
       <c r="D38" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>9.2742473233851409E-3</v>
       </c>
       <c r="E38" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>8.2884580787050896E-3</v>
       </c>
       <c r="F38" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>5.3045012487175002E-3</v>
       </c>
       <c r="G38" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.39753276850077E-3</v>
       </c>
       <c r="H38" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>3.8031744028528902E-3</v>
       </c>
       <c r="I38" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>3.4249250010206047E-3</v>
       </c>
       <c r="J38" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>3.0300490707755069E-3</v>
       </c>
       <c r="K38" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2.750517818215462E-3</v>
       </c>
       <c r="L38" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2.5108708257625678E-3</v>
       </c>
       <c r="M38" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2.299372229839061E-3</v>
       </c>
       <c r="N38" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2.107345768743038E-3</v>
       </c>
       <c r="O38" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1.930939174205478E-3</v>
       </c>
       <c r="P38" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1.7665083615798229E-3</v>
       </c>
       <c r="Q38" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1.611514314896446E-3</v>
       </c>
       <c r="R38" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1.464464244531832E-3</v>
       </c>
       <c r="S38" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1.3240858376809763E-3</v>
       </c>
       <c r="T38" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1.1894035666051008E-3</v>
       </c>
       <c r="U38" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1.0596098576443221E-3</v>
       </c>
       <c r="V38" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>9.3408257734605728E-4</v>
       </c>
     </row>
@@ -5392,83 +5229,83 @@
         <v>2.147407824905633E-3</v>
       </c>
       <c r="C50" s="2">
-        <f t="shared" ref="C50:V50" si="9">SUM(C46:C49)</f>
+        <f t="shared" ref="C50:V50" si="7">SUM(C46:C49)</f>
         <v>1.6233937867611065E-3</v>
       </c>
       <c r="D50" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1.3139225427367402E-3</v>
       </c>
       <c r="E50" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1.2646330805027373E-3</v>
       </c>
       <c r="F50" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1.1154352390033582E-3</v>
       </c>
       <c r="G50" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1.0700868149925212E-3</v>
       </c>
       <c r="H50" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1.0403688967101283E-3</v>
       </c>
       <c r="I50" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1.0214564266185133E-3</v>
       </c>
       <c r="J50" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1.0017126301062594E-3</v>
       </c>
       <c r="K50" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>9.8773606747825618E-4</v>
       </c>
       <c r="L50" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>9.7575371785561132E-4</v>
       </c>
       <c r="M50" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>9.6517878805943631E-4</v>
       </c>
       <c r="N50" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>9.5557746500463526E-4</v>
       </c>
       <c r="O50" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>9.467571352777571E-4</v>
       </c>
       <c r="P50" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>9.3853559464647442E-4</v>
       </c>
       <c r="Q50" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>9.3078589231230559E-4</v>
       </c>
       <c r="R50" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>9.2343338879407493E-4</v>
       </c>
       <c r="S50" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>9.1641446845153228E-4</v>
       </c>
       <c r="T50" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>9.0968035489773821E-4</v>
       </c>
       <c r="U50" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>9.0319066944969935E-4</v>
       </c>
       <c r="V50" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>8.9691430543478614E-4</v>
       </c>
     </row>
@@ -5548,88 +5385,266 @@
         <v>76</v>
       </c>
       <c r="B54" s="2">
-        <f>SUM(B24:B25,B28:B29,B36:B37,B41:B43,B46:B49,B52)</f>
+        <f>SUM(B24:B25,B27:B28,B36:B37,B41:B43,B46:B49,B52)</f>
         <v>0.11359588998916793</v>
       </c>
       <c r="C54" s="2">
-        <f>SUM(C24:C25,C28:C29,C36:C37,C41:C43,C46:C49,C52)</f>
+        <f>SUM(C24:C25,C27:C28,C36:C37,C41:C43,C46:C49,C52)</f>
         <v>7.5936664991725897E-2</v>
       </c>
       <c r="D54" s="2">
-        <f>SUM(D24:D25,D28:D29,D36:D37,D41:D43,D46:D49,D52)</f>
+        <f>SUM(D24:D25,D27:D28,D36:D37,D41:D43,D46:D49,D52)</f>
         <v>4.9805743257470454E-2</v>
       </c>
       <c r="E54" s="2">
-        <f>SUM(E24:E25,E28:E29,E36:E37,E41:E43,E46:E49,E52)</f>
+        <f>SUM(E24:E25,E27:E28,E36:E37,E41:E43,E46:E49,E52)</f>
         <v>3.8417186609800397E-2</v>
       </c>
       <c r="F54" s="2">
-        <f>SUM(F24:F25,F28:F29,F36:F37,F41:F43,F46:F49,F52)</f>
+        <f>SUM(F24:F25,F27:F28,F36:F37,F41:F43,F46:F49,F52)</f>
         <v>2.9361977068217162E-2</v>
       </c>
       <c r="G54" s="2">
-        <f>SUM(G24:G25,G28:G29,G36:G37,G41:G43,G46:G49,G52)</f>
+        <f>SUM(G24:G25,G27:G28,G36:G37,G41:G43,G46:G49,G52)</f>
         <v>2.566437127563612E-2</v>
       </c>
       <c r="H54" s="2">
-        <f>SUM(H24:H25,H28:H29,H36:H37,H41:H43,H46:H49,H52)</f>
+        <f>SUM(H24:H25,H27:H28,H36:H37,H41:H43,H46:H49,H52)</f>
         <v>2.3479153045517669E-2</v>
       </c>
       <c r="I54" s="2">
-        <f>SUM(I24:I25,I28:I29,I36:I37,I41:I43,I46:I49,I52)</f>
+        <f>SUM(I24:I25,I27:I28,I36:I37,I41:I43,I46:I49,I52)</f>
         <v>2.2160361513504225E-2</v>
       </c>
       <c r="J54" s="2">
-        <f>SUM(J24:J25,J28:J29,J36:J37,J41:J43,J46:J49,J52)</f>
+        <f>SUM(J24:J25,J27:J28,J36:J37,J41:J43,J46:J49,J52)</f>
         <v>2.1162741442653718E-2</v>
       </c>
       <c r="K54" s="2">
-        <f>SUM(K24:K25,K28:K29,K36:K37,K41:K43,K46:K49,K52)</f>
+        <f>SUM(K24:K25,K27:K28,K36:K37,K41:K43,K46:K49,K52)</f>
         <v>2.0402020013591659E-2</v>
       </c>
       <c r="L54" s="2">
-        <f>SUM(L24:L25,L28:L29,L36:L37,L41:L43,L46:L49,L52)</f>
+        <f>SUM(L24:L25,L27:L28,L36:L37,L41:L43,L46:L49,L52)</f>
         <v>1.9796966354995164E-2</v>
       </c>
       <c r="M54" s="2">
-        <f>SUM(M24:M25,M28:M29,M36:M37,M41:M43,M46:M49,M52)</f>
+        <f>SUM(M24:M25,M27:M28,M36:M37,M41:M43,M46:M49,M52)</f>
         <v>1.9289370095146738E-2</v>
       </c>
       <c r="N54" s="2">
-        <f>SUM(N24:N25,N28:N29,N36:N37,N41:N43,N46:N49,N52)</f>
+        <f>SUM(N24:N25,N27:N28,N36:N37,N41:N43,N46:N49,N52)</f>
         <v>1.8865876303766713E-2</v>
       </c>
       <c r="O54" s="2">
-        <f>SUM(O24:O25,O28:O29,O36:O37,O41:O43,O46:O49,O52)</f>
+        <f>SUM(O24:O25,O27:O28,O36:O37,O41:O43,O46:O49,O52)</f>
         <v>1.8507014253674504E-2</v>
       </c>
       <c r="P54" s="2">
-        <f>SUM(P24:P25,P28:P29,P36:P37,P41:P43,P46:P49,P52)</f>
+        <f>SUM(P24:P25,P27:P28,P36:P37,P41:P43,P46:P49,P52)</f>
         <v>1.81799343031823E-2</v>
       </c>
       <c r="Q54" s="2">
-        <f>SUM(Q24:Q25,Q28:Q29,Q36:Q37,Q41:Q43,Q46:Q49,Q52)</f>
+        <f>SUM(Q24:Q25,Q27:Q28,Q36:Q37,Q41:Q43,Q46:Q49,Q52)</f>
         <v>1.789563865223661E-2</v>
       </c>
       <c r="R54" s="2">
-        <f>SUM(R24:R25,R28:R29,R36:R37,R41:R43,R46:R49,R52)</f>
+        <f>SUM(R24:R25,R27:R28,R36:R37,R41:R43,R46:R49,R52)</f>
         <v>1.7637770629254389E-2</v>
       </c>
       <c r="S54" s="2">
-        <f>SUM(S24:S25,S28:S29,S36:S37,S41:S43,S46:S49,S52)</f>
+        <f>SUM(S24:S25,S27:S28,S36:S37,S41:S43,S46:S49,S52)</f>
         <v>1.7412269747100088E-2</v>
       </c>
       <c r="T54" s="2">
-        <f>SUM(T24:T25,T28:T29,T36:T37,T41:T43,T46:T49,T52)</f>
+        <f>SUM(T24:T25,T27:T28,T36:T37,T41:T43,T46:T49,T52)</f>
         <v>1.7181085772431704E-2</v>
       </c>
       <c r="U54" s="2">
-        <f>SUM(U24:U25,U28:U29,U36:U37,U41:U43,U46:U49,U52)</f>
+        <f>SUM(U24:U25,U27:U28,U36:U37,U41:U43,U46:U49,U52)</f>
         <v>1.6981082779185083E-2</v>
       </c>
       <c r="V54" s="2">
-        <f>SUM(V24:V25,V28:V29,V36:V37,V41:V43,V46:V49,V52)</f>
+        <f>SUM(V24:V25,V27:V28,V36:V37,V41:V43,V46:V49,V52)</f>
         <v>1.6779737928805567E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A55" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B55" s="2">
+        <f>SUM(B24:B25)</f>
+        <v>7.5956033152108748E-2</v>
+      </c>
+      <c r="C55" s="2">
+        <f>SUM(C24:C25)</f>
+        <v>5.0533256419405093E-2</v>
+      </c>
+      <c r="D55" s="2">
+        <f>SUM(D24:D25)</f>
+        <v>3.1545182759264739E-2</v>
+      </c>
+      <c r="E55" s="2">
+        <f>SUM(E24:E25)</f>
+        <v>2.1487520413685623E-2</v>
+      </c>
+      <c r="F55" s="2">
+        <f>SUM(F24:F25)</f>
+        <v>1.5836024451445274E-2</v>
+      </c>
+      <c r="G55" s="2">
+        <f>SUM(G24:G25)</f>
+        <v>1.3206980896168783E-2</v>
+      </c>
+      <c r="H55" s="2">
+        <f>SUM(H24:H25)</f>
+        <v>1.1731214972786497E-2</v>
+      </c>
+      <c r="I55" s="2">
+        <f>SUM(I24:I25)</f>
+        <v>1.0879538691473404E-2</v>
+      </c>
+      <c r="J55" s="2">
+        <f>SUM(J24:J25)</f>
+        <v>1.0359368847452102E-2</v>
+      </c>
+      <c r="K55" s="2">
+        <f>SUM(K24:K25)</f>
+        <v>9.9480185112243227E-3</v>
+      </c>
+      <c r="L55" s="2">
+        <f>SUM(L24:L25)</f>
+        <v>9.6461172407927252E-3</v>
+      </c>
+      <c r="M55" s="2">
+        <f>SUM(M24:M25)</f>
+        <v>9.4144742796864987E-3</v>
+      </c>
+      <c r="N55" s="2">
+        <f>SUM(N24:N25)</f>
+        <v>9.2461083148904066E-3</v>
+      </c>
+      <c r="O55" s="2">
+        <f>SUM(O24:O25)</f>
+        <v>9.1197186347101618E-3</v>
+      </c>
+      <c r="P55" s="2">
+        <f>SUM(P24:P25)</f>
+        <v>9.0155381666054395E-3</v>
+      </c>
+      <c r="Q55" s="2">
+        <f>SUM(Q24:Q25)</f>
+        <v>8.9442388080117861E-3</v>
+      </c>
+      <c r="R55" s="2">
+        <f>SUM(R24:R25)</f>
+        <v>8.8880342965425001E-3</v>
+      </c>
+      <c r="S55" s="2">
+        <f>SUM(S24:S25)</f>
+        <v>8.8603189023480754E-3</v>
+      </c>
+      <c r="T55" s="2">
+        <f>SUM(T24:T25)</f>
+        <v>8.8210273199181115E-3</v>
+      </c>
+      <c r="U55" s="2">
+        <f>SUM(U24:U25)</f>
+        <v>8.8017692048181113E-3</v>
+      </c>
+      <c r="V55" s="2">
+        <f>SUM(V24:V25)</f>
+        <v>8.7859108805507374E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A56" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56" s="2">
+        <f>SUM(B27:B28)</f>
+        <v>3.9924354393298276E-3</v>
+      </c>
+      <c r="C56" s="2">
+        <f>SUM(C27:C28)</f>
+        <v>2.8150319756265908E-3</v>
+      </c>
+      <c r="D56" s="2">
+        <f>SUM(D27:D28)</f>
+        <v>2.2258300260232147E-3</v>
+      </c>
+      <c r="E56" s="2">
+        <f>SUM(E27:E28)</f>
+        <v>1.9847644308463373E-3</v>
+      </c>
+      <c r="F56" s="2">
+        <f>SUM(F27:F28)</f>
+        <v>1.7689555229904227E-3</v>
+      </c>
+      <c r="G56" s="2">
+        <f>SUM(G27:G28)</f>
+        <v>1.7074601899134357E-3</v>
+      </c>
+      <c r="H56" s="2">
+        <f>SUM(H27:H28)</f>
+        <v>1.6768341671075397E-3</v>
+      </c>
+      <c r="I56" s="2">
+        <f>SUM(I27:I28)</f>
+        <v>1.6616307883310971E-3</v>
+      </c>
+      <c r="J56" s="2">
+        <f>SUM(J27:J28)</f>
+        <v>1.6535502882592396E-3</v>
+      </c>
+      <c r="K56" s="2">
+        <f>SUM(K27:K28)</f>
+        <v>1.6524370106130112E-3</v>
+      </c>
+      <c r="L56" s="2">
+        <f>SUM(L27:L28)</f>
+        <v>1.6556639645236505E-3</v>
+      </c>
+      <c r="M56" s="2">
+        <f>SUM(M27:M28)</f>
+        <v>1.6565341915011306E-3</v>
+      </c>
+      <c r="N56" s="2">
+        <f>SUM(N27:N28)</f>
+        <v>1.6577841490680238E-3</v>
+      </c>
+      <c r="O56" s="2">
+        <f>SUM(O27:O28)</f>
+        <v>1.6652887034204968E-3</v>
+      </c>
+      <c r="P56" s="2">
+        <f>SUM(P27:P28)</f>
+        <v>1.6697915742899521E-3</v>
+      </c>
+      <c r="Q56" s="2">
+        <f>SUM(Q27:Q28)</f>
+        <v>1.6742890309554607E-3</v>
+      </c>
+      <c r="R56" s="2">
+        <f>SUM(R27:R28)</f>
+        <v>1.6817780933253746E-3</v>
+      </c>
+      <c r="S56" s="2">
+        <f>SUM(S27:S28)</f>
+        <v>1.6861399325588937E-3</v>
+      </c>
+      <c r="T56" s="2">
+        <f>SUM(T27:T28)</f>
+        <v>1.6904139249501451E-3</v>
+      </c>
+      <c r="U56" s="2">
+        <f>SUM(U27:U28)</f>
+        <v>1.7007024412123398E-3</v>
+      </c>
+      <c r="V56" s="2">
+        <f>SUM(V27:V28)</f>
+        <v>1.7017695594133738E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Final Sizing Folder
</commit_message>
<xml_diff>
--- a/Wing Tail Drag Buildup/Drag.xlsx
+++ b/Wing Tail Drag Buildup/Drag.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EddieH\Documents\GitHub\Senior-Design\Wing Tail Drag Buildup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00DF19C-BEF7-4254-AB1D-06485ADAE56E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8D1D27-429B-45E1-ACE9-FD900AE7469A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{82617F0D-A785-403D-9CC0-085A46D2A0AD}"/>
+    <workbookView xWindow="-2768" yWindow="1500" windowWidth="22201" windowHeight="13605" xr2:uid="{82617F0D-A785-403D-9CC0-085A46D2A0AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="107">
   <si>
     <t>Range</t>
   </si>
@@ -525,17 +525,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -545,7 +538,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -563,6 +555,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3701,7 +3709,7 @@
   <dimension ref="A1:W61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4:J9"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3712,378 +3720,436 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="J1">
+      <c r="J1" s="4">
         <v>454.47840000000002</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="7">
+      <c r="O1" s="4">
         <v>2</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="8"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="5"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="35">
         <v>3.4009999999999998E-7</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="36" t="s">
         <v>27</v>
       </c>
       <c r="L2" s="2"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="11"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="8"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="A3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="27">
         <v>575</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="27">
         <v>18000</v>
       </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="32">
         <v>1.3546000000000001E-3</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="N3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="O3" s="10">
+      <c r="O3" s="7">
         <v>1</v>
       </c>
-      <c r="P3" s="10">
+      <c r="P3" s="7">
         <v>2</v>
       </c>
-      <c r="Q3" s="10">
+      <c r="Q3" s="7">
         <v>3</v>
       </c>
-      <c r="R3" s="10">
+      <c r="R3" s="7">
         <v>4</v>
       </c>
-      <c r="S3" s="11"/>
+      <c r="S3" s="8"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="I4" s="2" t="s">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="I4" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="32">
         <v>38.531999999999996</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="N4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="O4" s="10">
+      <c r="O4" s="7">
         <v>5.7469999999999999</v>
       </c>
-      <c r="P4" s="10">
+      <c r="P4" s="7">
         <v>4.9809999999999999</v>
       </c>
-      <c r="Q4" s="10">
+      <c r="Q4" s="7">
         <v>4.2144000000000004</v>
       </c>
-      <c r="R4" s="10">
+      <c r="R4" s="7">
         <v>3.4481999999999999</v>
       </c>
-      <c r="S4" s="11" t="s">
+      <c r="S4" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+      <c r="A5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="I5" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="32">
         <v>4.5975999999999999</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="N5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="10">
+      <c r="O5" s="7">
         <f>O4*0.25*($J$6/2)</f>
         <v>17.241</v>
       </c>
-      <c r="P5" s="10">
+      <c r="P5" s="7">
         <f t="shared" ref="P5:R5" si="0">P4*0.25*($J$6/2)</f>
         <v>14.943</v>
       </c>
-      <c r="Q5" s="10">
+      <c r="Q5" s="7">
         <f t="shared" si="0"/>
         <v>12.6432</v>
       </c>
-      <c r="R5" s="10">
+      <c r="R5" s="7">
         <f t="shared" si="0"/>
         <v>10.3446</v>
       </c>
-      <c r="S5" s="11" t="s">
+      <c r="S5" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="D6" s="2">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="27">
         <v>540</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="I6" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="32">
         <v>24</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="12" t="s">
+      <c r="N6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="O6" s="13">
+      <c r="O6" s="10">
         <f>($J$3*$O$20*O4)/$J$2</f>
         <v>4349098.4357541902</v>
       </c>
-      <c r="P6" s="13">
+      <c r="P6" s="10">
         <f>($J$3*$O$20*P4)/$J$2</f>
         <v>3769420.4469273747</v>
       </c>
-      <c r="Q6" s="13">
+      <c r="Q6" s="10">
         <f>($J$3*$O$20*Q4)/$J$2</f>
         <v>3189288.4022346372</v>
       </c>
-      <c r="R6" s="13">
+      <c r="R6" s="10">
         <f>($J$3*$O$20*R4)/$J$2</f>
         <v>2609459.061452514</v>
       </c>
-      <c r="S6" s="14"/>
+      <c r="S6" s="11"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="I7" t="s">
+      <c r="I7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="7">
         <v>3.0649999999999999</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="37" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="I8" t="s">
+      <c r="I8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="7">
         <v>6.13</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="37" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="38">
         <v>15</v>
       </c>
+      <c r="K9" s="11"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="E10" s="28" t="s">
         <v>38</v>
       </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="5"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+      <c r="A11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="7">
         <v>0.04</v>
       </c>
-      <c r="E11" t="s">
+      <c r="C11" s="8"/>
+      <c r="E11" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="7">
         <v>2.7799999999999998E-2</v>
       </c>
-      <c r="H11" t="s">
+      <c r="G11" s="7"/>
+      <c r="H11" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="7">
         <v>0.12075</v>
       </c>
-      <c r="K11" t="s">
+      <c r="J11" s="7"/>
+      <c r="K11" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="8">
         <v>0.02</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+      <c r="A12" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="7">
         <v>0</v>
       </c>
-      <c r="E12" t="s">
+      <c r="C12" s="8"/>
+      <c r="E12" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="7">
         <v>5.1190000000000003E-3</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="G12" s="7"/>
+      <c r="H12" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="32">
         <f>1.05*F14*I11</f>
         <v>0.11410875000000001</v>
       </c>
-      <c r="K12" t="s">
+      <c r="J12" s="7"/>
+      <c r="K12" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+      <c r="A13" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="29">
         <f>(1/J9)-(1/(1+J9)^1.7)</f>
         <v>5.7692460768252324E-2</v>
       </c>
-      <c r="E13" t="s">
+      <c r="C13" s="8"/>
+      <c r="E13" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="7">
         <f>(0.5*(F11-F12))/9</f>
         <v>1.2600555555555555E-3</v>
       </c>
-      <c r="H13" t="s">
+      <c r="G13" s="7"/>
+      <c r="H13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="7">
         <v>0</v>
       </c>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="8"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+      <c r="A14" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="29">
         <f>(10 -3*0.5)/7</f>
         <v>1.2142857142857142</v>
       </c>
-      <c r="E14" t="s">
+      <c r="C14" s="8"/>
+      <c r="E14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="7">
         <v>0.9</v>
       </c>
-      <c r="H14" t="s">
+      <c r="G14" s="7"/>
+      <c r="H14" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="7">
         <v>0.1026</v>
       </c>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="8"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+      <c r="A15" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="7">
         <v>1.25</v>
       </c>
-      <c r="H15" t="s">
+      <c r="C15" s="8"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="7">
         <v>2.8163</v>
       </c>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="8"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="31">
         <f>4.44*(B13*B14*B15)^1.19</f>
         <v>0.24478196964639271</v>
       </c>
-      <c r="H16" t="s">
+      <c r="C16" s="11"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="7">
         <v>11.547000000000001</v>
       </c>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="8"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="H17" t="s">
+      <c r="E17" s="9"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="33">
         <v>4.0999999999999996</v>
       </c>
+      <c r="J17" s="33"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="11"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
@@ -4091,2190 +4157,2190 @@
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="F20" s="20" t="s">
+      <c r="F20" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="G20" s="20" t="s">
+      <c r="G20" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="H20" s="20" t="s">
+      <c r="H20" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="I20" s="20" t="s">
+      <c r="I20" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="J20" s="20" t="s">
+      <c r="J20" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="K20" s="20" t="s">
+      <c r="K20" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="L20" s="20" t="s">
+      <c r="L20" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="M20" s="20" t="s">
+      <c r="M20" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="N20" s="20" t="s">
+      <c r="N20" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="O20" s="20" t="s">
+      <c r="O20" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="P20" s="20" t="s">
+      <c r="P20" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="Q20" s="20" t="s">
+      <c r="Q20" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="R20" s="20" t="s">
+      <c r="R20" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="S20" s="20" t="s">
+      <c r="S20" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="T20" s="20" t="s">
+      <c r="T20" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="U20" s="20" t="s">
+      <c r="U20" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="V20" s="20" t="s">
+      <c r="V20" s="16" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="21">
+      <c r="B21" s="17">
         <f>B20*1.68780986</f>
         <v>101.26859159999999</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C21" s="17">
         <f>C20*1.68780986</f>
         <v>118.14669019999999</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D21" s="17">
         <f t="shared" ref="D21:G21" si="1">D20*1.68780986</f>
         <v>135.02478880000001</v>
       </c>
-      <c r="E21" s="21">
+      <c r="E21" s="17">
         <f t="shared" si="1"/>
         <v>151.9028874</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21" s="17">
         <f t="shared" si="1"/>
         <v>168.78098600000001</v>
       </c>
-      <c r="G21" s="21">
+      <c r="G21" s="17">
         <f t="shared" si="1"/>
         <v>185.6590846</v>
       </c>
-      <c r="H21" s="21">
+      <c r="H21" s="17">
         <f>H20*1.68780986</f>
         <v>202.53718319999999</v>
       </c>
-      <c r="I21" s="21">
+      <c r="I21" s="17">
         <f t="shared" ref="I21:V21" si="2">I20*1.68780986</f>
         <v>219.4152818</v>
       </c>
-      <c r="J21" s="21">
+      <c r="J21" s="17">
         <f t="shared" si="2"/>
         <v>236.29338039999999</v>
       </c>
-      <c r="K21" s="21">
+      <c r="K21" s="17">
         <f t="shared" si="2"/>
         <v>253.17147900000001</v>
       </c>
-      <c r="L21" s="21">
+      <c r="L21" s="17">
         <f t="shared" si="2"/>
         <v>270.04957760000002</v>
       </c>
-      <c r="M21" s="21">
+      <c r="M21" s="17">
         <f t="shared" si="2"/>
         <v>286.92767620000001</v>
       </c>
-      <c r="N21" s="21">
+      <c r="N21" s="17">
         <f t="shared" si="2"/>
         <v>303.80577479999999</v>
       </c>
-      <c r="O21" s="21">
+      <c r="O21" s="17">
         <f t="shared" si="2"/>
         <v>320.68387339999998</v>
       </c>
-      <c r="P21" s="21">
+      <c r="P21" s="17">
         <f t="shared" si="2"/>
         <v>337.56197200000003</v>
       </c>
-      <c r="Q21" s="21">
+      <c r="Q21" s="17">
         <f t="shared" si="2"/>
         <v>354.44007060000001</v>
       </c>
-      <c r="R21" s="21">
+      <c r="R21" s="17">
         <f t="shared" si="2"/>
         <v>371.3181692</v>
       </c>
-      <c r="S21" s="21">
+      <c r="S21" s="17">
         <f t="shared" si="2"/>
         <v>388.19626779999999</v>
       </c>
-      <c r="T21" s="21">
+      <c r="T21" s="17">
         <f t="shared" si="2"/>
         <v>405.07436639999997</v>
       </c>
-      <c r="U21" s="21">
+      <c r="U21" s="17">
         <f t="shared" si="2"/>
         <v>421.95246500000002</v>
       </c>
-      <c r="V21" s="21">
+      <c r="V21" s="17">
         <f t="shared" si="2"/>
         <v>438.8305636</v>
       </c>
-      <c r="W21" s="16"/>
+      <c r="W21" s="12"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="20">
+      <c r="B22" s="16">
         <v>12.125500000000001</v>
       </c>
-      <c r="C22" s="20">
+      <c r="C22" s="16">
         <v>8.9417500000000008</v>
       </c>
-      <c r="D22" s="20">
+      <c r="D22" s="16">
         <v>6.0397499999999997</v>
       </c>
-      <c r="E22" s="20">
+      <c r="E22" s="16">
         <v>5.5709999999999997</v>
       </c>
-      <c r="F22" s="20">
+      <c r="F22" s="16">
         <v>3.07775</v>
       </c>
-      <c r="G22" s="20">
+      <c r="G22" s="16">
         <v>2.1127500000000001</v>
       </c>
-      <c r="H22" s="20">
+      <c r="H22" s="16">
         <v>1.4067499999999999</v>
       </c>
-      <c r="I22" s="20">
+      <c r="I22" s="16">
         <v>1.0002500000000001</v>
       </c>
-      <c r="J22" s="20">
+      <c r="J22" s="16">
         <v>0.43325000000000002</v>
       </c>
-      <c r="K22" s="20">
+      <c r="K22" s="16">
         <v>8.8749999999999996E-2</v>
       </c>
-      <c r="L22" s="20">
+      <c r="L22" s="16">
         <v>-0.1915</v>
       </c>
-      <c r="M22" s="20">
+      <c r="M22" s="16">
         <v>-0.42099999999999999</v>
       </c>
-      <c r="N22" s="20">
+      <c r="N22" s="16">
         <v>-0.61575000000000002</v>
       </c>
-      <c r="O22" s="20">
+      <c r="O22" s="16">
         <v>-0.77875000000000005</v>
       </c>
-      <c r="P22" s="20">
+      <c r="P22" s="16">
         <v>-0.91725000000000001</v>
       </c>
-      <c r="Q22" s="20">
+      <c r="Q22" s="16">
         <v>-1.0369999999999999</v>
       </c>
-      <c r="R22" s="20">
+      <c r="R22" s="16">
         <v>-1.14025</v>
       </c>
-      <c r="S22" s="20">
+      <c r="S22" s="16">
         <v>-1.2297499999999999</v>
       </c>
-      <c r="T22" s="20">
+      <c r="T22" s="16">
         <v>-1.30775</v>
       </c>
-      <c r="U22" s="20">
+      <c r="U22" s="16">
         <v>-1.3765000000000001</v>
       </c>
-      <c r="V22" s="20">
+      <c r="V22" s="16">
         <v>-1.4377500000000001</v>
       </c>
-      <c r="W22" s="17" t="s">
+      <c r="W22" s="13" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="23">
+      <c r="B23" s="19">
         <v>1.5</v>
       </c>
-      <c r="C23" s="23">
+      <c r="C23" s="19">
         <f t="shared" ref="C23:V23" si="3" xml:space="preserve"> $D$6/(0.5*$J$3*C21^2*$J$4)</f>
         <v>1.4823406325816004</v>
       </c>
-      <c r="D23" s="23">
+      <c r="D23" s="19">
         <f t="shared" si="3"/>
         <v>1.1349170468202876</v>
       </c>
-      <c r="E23" s="23">
+      <c r="E23" s="19">
         <f t="shared" si="3"/>
         <v>0.89672458020368406</v>
       </c>
-      <c r="F23" s="23">
+      <c r="F23" s="19">
         <f t="shared" si="3"/>
         <v>0.72634690996498397</v>
       </c>
-      <c r="G23" s="23">
+      <c r="G23" s="19">
         <f t="shared" si="3"/>
         <v>0.60028670245040006</v>
       </c>
-      <c r="H23" s="23">
+      <c r="H23" s="19">
         <f t="shared" si="3"/>
         <v>0.50440757636457234</v>
       </c>
-      <c r="I23" s="23">
+      <c r="I23" s="19">
         <f t="shared" si="3"/>
         <v>0.42979107098519775</v>
       </c>
-      <c r="J23" s="23">
+      <c r="J23" s="19">
         <f t="shared" si="3"/>
         <v>0.37058515814540011</v>
       </c>
-      <c r="K23" s="23">
+      <c r="K23" s="19">
         <f t="shared" si="3"/>
         <v>0.32282084887332624</v>
       </c>
-      <c r="L23" s="23">
+      <c r="L23" s="19">
         <f t="shared" si="3"/>
         <v>0.2837292617050719</v>
       </c>
-      <c r="M23" s="23">
+      <c r="M23" s="19">
         <f t="shared" si="3"/>
         <v>0.25133111071452735</v>
       </c>
-      <c r="N23" s="23">
+      <c r="N23" s="19">
         <f t="shared" si="3"/>
         <v>0.22418114505092102</v>
       </c>
-      <c r="O23" s="23">
+      <c r="O23" s="19">
         <f t="shared" si="3"/>
         <v>0.20120413018420613</v>
       </c>
-      <c r="P23" s="23">
+      <c r="P23" s="19">
         <f t="shared" si="3"/>
         <v>0.18158672749124599</v>
       </c>
-      <c r="Q23" s="23">
+      <c r="Q23" s="19">
         <f t="shared" si="3"/>
         <v>0.16470451473128891</v>
       </c>
-      <c r="R23" s="23">
+      <c r="R23" s="19">
         <f t="shared" si="3"/>
         <v>0.15007167561260001</v>
       </c>
-      <c r="S23" s="23">
+      <c r="S23" s="19">
         <f t="shared" si="3"/>
         <v>0.13730565405765294</v>
       </c>
-      <c r="T23" s="23">
+      <c r="T23" s="19">
         <f t="shared" si="3"/>
         <v>0.12610189409114309</v>
       </c>
-      <c r="U23" s="23">
+      <c r="U23" s="19">
         <f t="shared" si="3"/>
         <v>0.11621550559439746</v>
       </c>
-      <c r="V23" s="23">
+      <c r="V23" s="19">
         <f t="shared" si="3"/>
         <v>0.10744776774629944</v>
       </c>
-      <c r="W23" s="17" t="s">
+      <c r="W23" s="13" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="23">
+      <c r="B24" s="19">
         <f t="shared" ref="B24:V24" si="4">((1+$B$11)*(B23^2))/(PI()*$J$9)</f>
         <v>4.9656342244671345E-2</v>
       </c>
-      <c r="C24" s="23">
+      <c r="C24" s="19">
         <f t="shared" si="4"/>
         <v>4.8494025229130482E-2</v>
       </c>
-      <c r="D24" s="23">
+      <c r="D24" s="19">
         <f t="shared" si="4"/>
         <v>2.842630726932184E-2</v>
       </c>
-      <c r="E24" s="23">
+      <c r="E24" s="19">
         <f t="shared" si="4"/>
         <v>1.7746403684673413E-2</v>
       </c>
-      <c r="F24" s="23">
+      <c r="F24" s="19">
         <f t="shared" si="4"/>
         <v>1.1643415457514223E-2</v>
       </c>
-      <c r="G24" s="23">
+      <c r="G24" s="19">
         <f t="shared" si="4"/>
         <v>7.9526094238878669E-3</v>
       </c>
-      <c r="H24" s="23">
+      <c r="H24" s="19">
         <f t="shared" si="4"/>
         <v>5.615073040853698E-3</v>
       </c>
-      <c r="I24" s="23">
+      <c r="I24" s="19">
         <f t="shared" si="4"/>
         <v>4.0766833995708237E-3</v>
       </c>
-      <c r="J24" s="23">
+      <c r="J24" s="19">
         <f t="shared" si="4"/>
         <v>3.0308765768206551E-3</v>
       </c>
-      <c r="K24" s="23">
+      <c r="K24" s="19">
         <f t="shared" si="4"/>
         <v>2.2999339175336737E-3</v>
       </c>
-      <c r="L24" s="23">
+      <c r="L24" s="19">
         <f t="shared" si="4"/>
         <v>1.776644204332615E-3</v>
       </c>
-      <c r="M24" s="23">
+      <c r="M24" s="19">
         <f t="shared" si="4"/>
         <v>1.3940704083421206E-3</v>
       </c>
-      <c r="N24" s="23">
+      <c r="N24" s="19">
         <f t="shared" si="4"/>
         <v>1.1091502302920883E-3</v>
       </c>
-      <c r="O24" s="23">
+      <c r="O24" s="19">
         <f t="shared" si="4"/>
         <v>8.9344123030933055E-4</v>
       </c>
-      <c r="P24" s="23">
+      <c r="P24" s="19">
         <f t="shared" si="4"/>
         <v>7.2771346609463896E-4</v>
       </c>
-      <c r="Q24" s="23">
+      <c r="Q24" s="19">
         <f t="shared" si="4"/>
         <v>5.9869166949543797E-4</v>
       </c>
-      <c r="R24" s="23">
+      <c r="R24" s="19">
         <f t="shared" si="4"/>
         <v>4.9703808899299168E-4</v>
       </c>
-      <c r="S24" s="23">
+      <c r="S24" s="19">
         <f t="shared" si="4"/>
         <v>4.1607253610136558E-4</v>
       </c>
-      <c r="T24" s="23">
+      <c r="T24" s="19">
         <f t="shared" si="4"/>
         <v>3.5094206505335612E-4</v>
       </c>
-      <c r="U24" s="23">
+      <c r="U24" s="19">
         <f t="shared" si="4"/>
         <v>2.980714357123642E-4</v>
       </c>
-      <c r="V24" s="23">
+      <c r="V24" s="19">
         <f t="shared" si="4"/>
         <v>2.5479271247317648E-4</v>
       </c>
-      <c r="W24" s="17" t="s">
+      <c r="W24" s="13" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="23">
+      <c r="B25" s="19">
         <v>2.62996909074374E-2</v>
       </c>
-      <c r="C25" s="23">
+      <c r="C25" s="19">
         <v>1.86289773519932E-2</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25" s="19">
         <v>1.2843480112571399E-2</v>
       </c>
-      <c r="E25" s="23">
+      <c r="E25" s="19">
         <v>9.8121395203986297E-3</v>
       </c>
-      <c r="F25" s="23">
+      <c r="F25" s="19">
         <v>8.1758070473596806E-3</v>
       </c>
-      <c r="G25" s="23">
+      <c r="G25" s="19">
         <v>7.9749493381566297E-3</v>
       </c>
-      <c r="H25" s="23">
+      <c r="H25" s="19">
         <v>8.0370514870199104E-3</v>
       </c>
-      <c r="I25" s="23">
+      <c r="I25" s="19">
         <v>8.1974836499532893E-3</v>
       </c>
-      <c r="J25" s="23">
+      <c r="J25" s="19">
         <v>8.3653514057388592E-3</v>
       </c>
-      <c r="K25" s="23">
+      <c r="K25" s="19">
         <v>8.4348891474543292E-3</v>
       </c>
-      <c r="L25" s="23">
+      <c r="L25" s="19">
         <v>8.4772608253743907E-3</v>
       </c>
-      <c r="M25" s="23">
+      <c r="M25" s="19">
         <v>8.4973136369636392E-3</v>
       </c>
-      <c r="N25" s="23">
+      <c r="N25" s="19">
         <v>8.51639700905997E-3</v>
       </c>
-      <c r="O25" s="23">
+      <c r="O25" s="19">
         <v>8.5319225462757893E-3</v>
       </c>
-      <c r="P25" s="23">
+      <c r="P25" s="19">
         <v>8.5367745788500898E-3</v>
       </c>
-      <c r="Q25" s="23">
+      <c r="Q25" s="19">
         <v>8.5503588195252195E-3</v>
       </c>
-      <c r="R25" s="23">
+      <c r="R25" s="19">
         <v>8.56103232416674E-3</v>
       </c>
-      <c r="S25" s="23">
+      <c r="S25" s="19">
         <v>8.5865842671771896E-3</v>
       </c>
-      <c r="T25" s="23">
+      <c r="T25" s="19">
         <v>8.5901421020576994E-3</v>
       </c>
-      <c r="U25" s="23">
+      <c r="U25" s="19">
         <v>8.6056676392735204E-3</v>
       </c>
-      <c r="V25" s="23">
+      <c r="V25" s="19">
         <v>8.6182824404557306E-3</v>
       </c>
-      <c r="W25" s="17" t="s">
+      <c r="W25" s="13" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="23">
+      <c r="B26" s="19">
         <f t="shared" ref="B26:V26" si="5">$I$12*B22*(1-$B$16)*$I$14</f>
         <v>0.10721074516785122</v>
       </c>
-      <c r="C26" s="23">
+      <c r="C26" s="19">
         <f t="shared" si="5"/>
         <v>7.9060795893335006E-2</v>
       </c>
-      <c r="D26" s="23">
+      <c r="D26" s="19">
         <f t="shared" si="5"/>
         <v>5.340201213372886E-2</v>
       </c>
-      <c r="E26" s="23">
+      <c r="E26" s="19">
         <f t="shared" si="5"/>
         <v>4.925743774113224E-2</v>
       </c>
-      <c r="F26" s="23">
+      <c r="F26" s="19">
         <f t="shared" si="5"/>
         <v>2.7212722851870357E-2</v>
       </c>
-      <c r="G26" s="23">
+      <c r="G26" s="19">
         <f t="shared" si="5"/>
         <v>1.8680425702311463E-2</v>
       </c>
-      <c r="H26" s="23">
+      <c r="H26" s="19">
         <f t="shared" si="5"/>
         <v>1.2438144057141946E-2</v>
       </c>
-      <c r="I26" s="23">
+      <c r="I26" s="19">
         <f t="shared" si="5"/>
         <v>8.843969143882165E-3</v>
       </c>
-      <c r="J26" s="23">
+      <c r="J26" s="19">
         <f t="shared" si="5"/>
         <v>3.8306919585972977E-3</v>
       </c>
-      <c r="K26" s="23">
+      <c r="K26" s="19">
         <f t="shared" si="5"/>
         <v>7.8470608499829229E-4</v>
       </c>
-      <c r="L26" s="23">
+      <c r="L26" s="19">
         <f t="shared" si="5"/>
         <v>-1.6931967918554704E-3</v>
       </c>
-      <c r="M26" s="23">
+      <c r="M26" s="19">
         <f t="shared" si="5"/>
         <v>-3.7223804144707728E-3</v>
       </c>
-      <c r="N26" s="23">
+      <c r="N26" s="19">
         <f t="shared" si="5"/>
         <v>-5.4443129221149128E-3</v>
       </c>
-      <c r="O26" s="23">
+      <c r="O26" s="19">
         <f t="shared" si="5"/>
         <v>-6.8855195909005105E-3</v>
       </c>
-      <c r="P26" s="23">
+      <c r="P26" s="19">
         <f t="shared" si="5"/>
         <v>-8.1101031714330557E-3</v>
       </c>
-      <c r="Q26" s="23">
+      <c r="Q26" s="19">
         <f t="shared" si="5"/>
         <v>-9.168903776261738E-3</v>
       </c>
-      <c r="R26" s="23">
+      <c r="R26" s="19">
         <f t="shared" si="5"/>
         <v>-1.0081815362471018E-2</v>
       </c>
-      <c r="S26" s="23">
+      <c r="S26" s="19">
         <f t="shared" si="5"/>
         <v>-1.0873152766497465E-2</v>
       </c>
-      <c r="T26" s="23">
+      <c r="T26" s="19">
         <f t="shared" si="5"/>
         <v>-1.1562809945425542E-2</v>
       </c>
-      <c r="U26" s="23">
+      <c r="U26" s="19">
         <f t="shared" si="5"/>
         <v>-1.2170680856339712E-2</v>
       </c>
-      <c r="V26" s="23">
+      <c r="V26" s="19">
         <f t="shared" si="5"/>
         <v>-1.2712238576972339E-2</v>
       </c>
-      <c r="W26" s="17" t="s">
+      <c r="W26" s="13" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="25">
+      <c r="B27" s="21">
         <f>((1+$L$11)*(B26^2))/(PI()*$I$17)</f>
         <v>9.102130786945075E-4</v>
       </c>
-      <c r="C27" s="25">
+      <c r="C27" s="21">
         <f>((1+$L$11)*(C26^2))/(PI()*$I$17)</f>
         <v>4.949813164342304E-4</v>
       </c>
-      <c r="D27" s="25">
+      <c r="D27" s="21">
         <f t="shared" ref="D27:V27" si="6">((1+$L$11)*(D26^2))/(PI()*$I$17)</f>
         <v>2.2583002602321459E-4</v>
       </c>
-      <c r="E27" s="25">
+      <c r="E27" s="21">
         <f t="shared" si="6"/>
         <v>1.9213658905250746E-4</v>
       </c>
-      <c r="F27" s="25">
+      <c r="F27" s="21">
         <f t="shared" si="6"/>
         <v>5.8642224952432596E-5</v>
       </c>
-      <c r="G27" s="25">
+      <c r="G27" s="21">
         <f t="shared" si="6"/>
         <v>2.7633759933155704E-5</v>
       </c>
-      <c r="H27" s="25">
+      <c r="H27" s="21">
         <f t="shared" si="6"/>
         <v>1.2251171156119612E-5</v>
       </c>
-      <c r="I27" s="25">
+      <c r="I27" s="21">
         <f t="shared" si="6"/>
         <v>6.1938527969972284E-6</v>
       </c>
-      <c r="J27" s="25">
+      <c r="J27" s="21">
         <f t="shared" si="6"/>
         <v>1.162039530909637E-6</v>
       </c>
-      <c r="K27" s="25">
+      <c r="K27" s="21">
         <f t="shared" si="6"/>
         <v>4.8761884681389963E-8</v>
       </c>
-      <c r="L27" s="25">
+      <c r="L27" s="21">
         <f t="shared" si="6"/>
         <v>2.2702898955059437E-7</v>
       </c>
-      <c r="M27" s="25">
+      <c r="M27" s="21">
         <f t="shared" si="6"/>
         <v>1.0972559670305719E-6</v>
       </c>
-      <c r="N27" s="25">
+      <c r="N27" s="21">
         <f t="shared" si="6"/>
         <v>2.3472135339238957E-6</v>
       </c>
-      <c r="O27" s="25">
+      <c r="O27" s="21">
         <f t="shared" si="6"/>
         <v>3.7543942748468985E-6</v>
       </c>
-      <c r="P27" s="25">
+      <c r="P27" s="21">
         <f t="shared" si="6"/>
         <v>5.2085783385320108E-6</v>
       </c>
-      <c r="Q27" s="25">
+      <c r="Q27" s="21">
         <f t="shared" si="6"/>
         <v>6.6573481982707112E-6</v>
       </c>
-      <c r="R27" s="25">
+      <c r="R27" s="21">
         <f t="shared" si="6"/>
         <v>8.049036956644549E-6</v>
       </c>
-      <c r="S27" s="25">
+      <c r="S27" s="21">
         <f t="shared" si="6"/>
         <v>9.362189384393714E-6</v>
       </c>
-      <c r="T27" s="25">
+      <c r="T27" s="21">
         <f t="shared" si="6"/>
         <v>1.0587494969865056E-5</v>
       </c>
-      <c r="U27" s="25">
+      <c r="U27" s="21">
         <f t="shared" si="6"/>
         <v>1.1729950814749983E-5</v>
       </c>
-      <c r="V27" s="25">
+      <c r="V27" s="21">
         <f t="shared" si="6"/>
         <v>1.2797069015783988E-5</v>
       </c>
-      <c r="W27" s="17" t="s">
+      <c r="W27" s="13" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="23">
+      <c r="B28" s="19">
         <v>3.0822223606353201E-3</v>
       </c>
-      <c r="C28" s="23">
+      <c r="C28" s="19">
         <v>2.3200506591923601E-3</v>
       </c>
-      <c r="D28" s="23">
+      <c r="D28" s="19">
         <v>2E-3</v>
       </c>
-      <c r="E28" s="23">
+      <c r="E28" s="19">
         <v>1.7926278417938299E-3</v>
       </c>
-      <c r="F28" s="23">
+      <c r="F28" s="19">
         <v>1.7103132980379901E-3</v>
       </c>
-      <c r="G28" s="23">
+      <c r="G28" s="19">
         <v>1.67982642998028E-3</v>
       </c>
-      <c r="H28" s="23">
+      <c r="H28" s="19">
         <v>1.66458299595142E-3</v>
       </c>
-      <c r="I28" s="23">
+      <c r="I28" s="19">
         <v>1.6554369355341E-3</v>
       </c>
-      <c r="J28" s="23">
+      <c r="J28" s="19">
         <v>1.6523882487283299E-3</v>
       </c>
-      <c r="K28" s="23">
+      <c r="K28" s="19">
         <v>1.6523882487283299E-3</v>
       </c>
-      <c r="L28" s="23">
+      <c r="L28" s="19">
         <v>1.6554369355341E-3</v>
       </c>
-      <c r="M28" s="23">
+      <c r="M28" s="19">
         <v>1.6554369355341E-3</v>
       </c>
-      <c r="N28" s="23">
+      <c r="N28" s="19">
         <v>1.6554369355341E-3</v>
       </c>
-      <c r="O28" s="23">
+      <c r="O28" s="19">
         <v>1.6615343091456499E-3</v>
       </c>
-      <c r="P28" s="23">
+      <c r="P28" s="19">
         <v>1.66458299595142E-3</v>
       </c>
-      <c r="Q28" s="23">
+      <c r="Q28" s="19">
         <v>1.6676316827571899E-3</v>
       </c>
-      <c r="R28" s="23">
+      <c r="R28" s="19">
         <v>1.6737290563687301E-3</v>
       </c>
-      <c r="S28" s="23">
+      <c r="S28" s="19">
         <v>1.6767777431745E-3</v>
       </c>
-      <c r="T28" s="23">
+      <c r="T28" s="19">
         <v>1.67982642998028E-3</v>
       </c>
-      <c r="U28" s="23">
+      <c r="U28" s="19">
         <v>1.6889724903975899E-3</v>
       </c>
-      <c r="V28" s="23">
+      <c r="V28" s="19">
         <v>1.6889724903975899E-3</v>
       </c>
-      <c r="W28" s="17" t="s">
+      <c r="W28" s="13" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="B29" s="23">
+      <c r="B29" s="19">
         <v>1.71032388663968E-3</v>
       </c>
-      <c r="C29" s="23">
+      <c r="C29" s="19">
         <v>1.6829933561714899E-3</v>
       </c>
-      <c r="D29" s="23">
+      <c r="D29" s="19">
         <v>1.66646942800789E-3</v>
       </c>
-      <c r="E29" s="23">
+      <c r="E29" s="19">
         <v>1.65707204401536E-3</v>
       </c>
-      <c r="F29" s="23">
+      <c r="F29" s="19">
         <v>1.6508071213536799E-3</v>
       </c>
-      <c r="G29" s="23">
+      <c r="G29" s="19">
         <v>1.6445421986920001E-3</v>
       </c>
-      <c r="H29" s="23">
+      <c r="H29" s="19">
         <v>1.64054811585176E-3</v>
       </c>
-      <c r="I29" s="23">
+      <c r="I29" s="19">
         <v>1.63514481469947E-3</v>
       </c>
-      <c r="J29" s="23">
+      <c r="J29" s="19">
         <v>1.63514481469947E-3</v>
       </c>
-      <c r="K29" s="23">
+      <c r="K29" s="19">
         <v>1.63827727603031E-3</v>
       </c>
-      <c r="L29" s="23">
+      <c r="L29" s="19">
         <v>1.63514481469947E-3</v>
       </c>
-      <c r="M29" s="23">
+      <c r="M29" s="19">
         <v>1.63514481469947E-3</v>
       </c>
-      <c r="N29" s="23">
+      <c r="N29" s="19">
         <v>1.6414097373611499E-3</v>
       </c>
-      <c r="O29" s="23">
+      <c r="O29" s="19">
         <v>1.63827727603031E-3</v>
       </c>
-      <c r="P29" s="23">
+      <c r="P29" s="19">
         <v>1.6422713588705501E-3</v>
       </c>
-      <c r="Q29" s="23">
+      <c r="Q29" s="19">
         <v>1.6414097373611499E-3</v>
       </c>
-      <c r="R29" s="23">
+      <c r="R29" s="19">
         <v>1.64767466002284E-3</v>
       </c>
-      <c r="S29" s="23">
+      <c r="S29" s="19">
         <v>1.6445421986920001E-3</v>
       </c>
-      <c r="T29" s="23">
+      <c r="T29" s="19">
         <v>1.6539395826845201E-3</v>
       </c>
-      <c r="U29" s="23">
+      <c r="U29" s="19">
         <v>1.6508071213536799E-3</v>
       </c>
-      <c r="V29" s="23">
+      <c r="V29" s="19">
         <v>1.66020450534621E-3</v>
       </c>
-      <c r="W29" s="17" t="s">
+      <c r="W29" s="13" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A30" s="19"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="20"/>
-      <c r="M30" s="20"/>
-      <c r="N30" s="20"/>
-      <c r="O30" s="20"/>
-      <c r="P30" s="20"/>
-      <c r="Q30" s="20"/>
-      <c r="R30" s="20"/>
-      <c r="S30" s="20"/>
-      <c r="T30" s="20"/>
-      <c r="U30" s="20"/>
-      <c r="V30" s="20"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="16"/>
+      <c r="R30" s="16"/>
+      <c r="S30" s="16"/>
+      <c r="T30" s="16"/>
+      <c r="U30" s="16"/>
+      <c r="V30" s="16"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A31" s="19"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="20"/>
-      <c r="O31" s="20"/>
-      <c r="P31" s="20"/>
-      <c r="Q31" s="20"/>
-      <c r="R31" s="20"/>
-      <c r="S31" s="20"/>
-      <c r="T31" s="20"/>
-      <c r="U31" s="20"/>
-      <c r="V31" s="20"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="16"/>
+      <c r="R31" s="16"/>
+      <c r="S31" s="16"/>
+      <c r="T31" s="16"/>
+      <c r="U31" s="16"/>
+      <c r="V31" s="16"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A32" s="19"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="20"/>
-      <c r="M32" s="20"/>
-      <c r="N32" s="20"/>
-      <c r="O32" s="20"/>
-      <c r="P32" s="20"/>
-      <c r="Q32" s="20"/>
-      <c r="R32" s="20"/>
-      <c r="S32" s="20"/>
-      <c r="T32" s="20"/>
-      <c r="U32" s="20"/>
-      <c r="V32" s="20"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="16"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="16"/>
+      <c r="Q32" s="16"/>
+      <c r="R32" s="16"/>
+      <c r="S32" s="16"/>
+      <c r="T32" s="16"/>
+      <c r="U32" s="16"/>
+      <c r="V32" s="16"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A33" s="22" t="s">
+      <c r="A33" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="20"/>
-      <c r="M33" s="20"/>
-      <c r="N33" s="20"/>
-      <c r="O33" s="20"/>
-      <c r="P33" s="20"/>
-      <c r="Q33" s="20"/>
-      <c r="R33" s="20"/>
-      <c r="S33" s="20"/>
-      <c r="T33" s="20"/>
-      <c r="U33" s="20"/>
-      <c r="V33" s="20"/>
-      <c r="W33" s="30"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="16"/>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="16"/>
+      <c r="S33" s="16"/>
+      <c r="T33" s="16"/>
+      <c r="U33" s="16"/>
+      <c r="V33" s="16"/>
+      <c r="W33" s="26"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A34" s="26"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="20"/>
-      <c r="M34" s="20"/>
-      <c r="N34" s="20"/>
-      <c r="O34" s="20"/>
-      <c r="P34" s="20"/>
-      <c r="Q34" s="20"/>
-      <c r="R34" s="20"/>
-      <c r="S34" s="20"/>
-      <c r="T34" s="20"/>
-      <c r="U34" s="20"/>
-      <c r="V34" s="20"/>
+      <c r="A34" s="22"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="16"/>
+      <c r="R34" s="16"/>
+      <c r="S34" s="16"/>
+      <c r="T34" s="16"/>
+      <c r="U34" s="16"/>
+      <c r="V34" s="16"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="B35" s="23">
+      <c r="B35" s="19">
         <v>8.0654190909297693E-2</v>
       </c>
-      <c r="C35" s="23">
+      <c r="C35" s="19">
         <v>5.3919245662328502E-2</v>
       </c>
-      <c r="D35" s="23">
+      <c r="D35" s="19">
         <v>3.4075683804960198E-2</v>
       </c>
-      <c r="E35" s="23">
+      <c r="E35" s="19">
         <v>3.1260926619361099E-2</v>
       </c>
-      <c r="F35" s="23">
+      <c r="F35" s="19">
         <v>1.8260445654951302E-2</v>
       </c>
-      <c r="G35" s="23">
+      <c r="G35" s="19">
         <v>1.4080239068873899E-2</v>
       </c>
-      <c r="H35" s="23">
+      <c r="H35" s="19">
         <v>1.1325094853749801E-2</v>
       </c>
-      <c r="I35" s="23">
+      <c r="I35" s="19">
         <v>9.8549152115527706E-3</v>
       </c>
-      <c r="J35" s="23">
+      <c r="J35" s="19">
         <v>7.9469040624510993E-3</v>
       </c>
-      <c r="K35" s="23">
+      <c r="K35" s="19">
         <v>6.86847186683354E-3</v>
       </c>
-      <c r="L35" s="23">
+      <c r="L35" s="19">
         <v>6.0363530817529598E-3</v>
       </c>
-      <c r="M35" s="23">
+      <c r="M35" s="19">
         <v>5.3851349401790099E-3</v>
       </c>
-      <c r="N35" s="23">
+      <c r="N35" s="19">
         <v>4.8538720110385698E-3</v>
       </c>
-      <c r="O35" s="23">
+      <c r="O35" s="19">
         <v>4.4243007935562198E-3</v>
       </c>
-      <c r="P35" s="23">
+      <c r="P35" s="19">
         <v>4.0701023524739302E-3</v>
       </c>
-      <c r="Q35" s="23">
+      <c r="Q35" s="19">
         <v>3.7718605998456399E-3</v>
       </c>
-      <c r="R35" s="23">
+      <c r="R35" s="19">
         <v>3.5206781034025502E-3</v>
       </c>
-      <c r="S35" s="23">
+      <c r="S35" s="19">
         <v>3.3074189999513599E-3</v>
       </c>
-      <c r="T35" s="23">
+      <c r="T35" s="19">
         <v>3.1249522691504301E-3</v>
       </c>
-      <c r="U35" s="23">
+      <c r="U35" s="19">
         <v>2.9667436566930901E-3</v>
       </c>
-      <c r="V35" s="23">
+      <c r="V35" s="19">
         <v>2.82786222825106E-3</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="23">
+      <c r="B36" s="19">
         <v>2.1235574544969799E-2</v>
       </c>
-      <c r="C36" s="23">
+      <c r="C36" s="19">
         <v>1.1200360436934001E-2</v>
       </c>
-      <c r="D36" s="23">
+      <c r="D36" s="19">
         <v>5.3524472121662704E-3</v>
       </c>
-      <c r="E36" s="23">
+      <c r="E36" s="19">
         <v>4.6545656112223204E-3</v>
       </c>
-      <c r="F36" s="23">
+      <c r="F36" s="19">
         <v>1.92426050732076E-3</v>
       </c>
-      <c r="G36" s="23">
+      <c r="G36" s="19">
         <v>1.2466107162451901E-3</v>
       </c>
-      <c r="H36" s="23">
+      <c r="H36" s="19">
         <v>8.6313264908666003E-4</v>
       </c>
-      <c r="I36" s="23">
+      <c r="I36" s="19">
         <v>6.8116584324750499E-4</v>
       </c>
-      <c r="J36" s="23">
+      <c r="J36" s="19">
         <v>4.7064255760330702E-4</v>
       </c>
-      <c r="K36" s="23">
+      <c r="K36" s="19">
         <v>3.65476371592562E-4</v>
       </c>
-      <c r="L36" s="23">
+      <c r="L36" s="19">
         <v>2.9167320261376799E-4</v>
       </c>
-      <c r="M36" s="23">
+      <c r="M36" s="19">
         <v>2.3863638350522101E-4</v>
       </c>
-      <c r="N36" s="23">
+      <c r="N36" s="19">
         <v>1.9859559567173799E-4</v>
       </c>
-      <c r="O36" s="23">
+      <c r="O36" s="19">
         <v>1.6843310603254801E-4</v>
       </c>
-      <c r="P36" s="23">
+      <c r="P36" s="19">
         <v>1.4511019225452301E-4</v>
       </c>
-      <c r="Q36" s="23">
+      <c r="Q36" s="19">
         <v>1.2659375603480601E-4</v>
       </c>
-      <c r="R36" s="23">
+      <c r="R36" s="19">
         <v>1.11818951292982E-4</v>
       </c>
-      <c r="S36" s="23">
+      <c r="S36" s="19">
         <v>9.9879289073276096E-5</v>
       </c>
-      <c r="T36" s="23">
+      <c r="T36" s="19">
         <v>9.0114881594810796E-5</v>
       </c>
-      <c r="U36" s="23">
+      <c r="U36" s="19">
         <v>8.1992750954734103E-5</v>
       </c>
-      <c r="V36" s="23">
+      <c r="V36" s="19">
         <v>7.5131420037182305E-5</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B37" s="23">
+      <c r="B37" s="19">
         <v>4.7083784217933399E-3</v>
       </c>
-      <c r="C37" s="23">
+      <c r="C37" s="19">
         <v>4.2633117669385002E-3</v>
       </c>
-      <c r="D37" s="23">
+      <c r="D37" s="19">
         <v>3.9218001112188696E-3</v>
       </c>
-      <c r="E37" s="23">
+      <c r="E37" s="19">
         <v>3.6338924674827701E-3</v>
       </c>
-      <c r="F37" s="23">
+      <c r="F37" s="19">
         <v>3.3802407413967401E-3</v>
       </c>
-      <c r="G37" s="23">
+      <c r="G37" s="19">
         <v>3.1509220522555801E-3</v>
       </c>
-      <c r="H37" s="23">
+      <c r="H37" s="19">
         <v>2.94004175376623E-3</v>
       </c>
-      <c r="I37" s="23">
+      <c r="I37" s="19">
         <v>2.7437591577730998E-3</v>
       </c>
-      <c r="J37" s="23">
+      <c r="J37" s="19">
         <v>2.5594065131721998E-3</v>
       </c>
-      <c r="K37" s="23">
+      <c r="K37" s="19">
         <v>2.3850414466229002E-3</v>
       </c>
-      <c r="L37" s="23">
+      <c r="L37" s="19">
         <v>2.2191976231487999E-3</v>
       </c>
-      <c r="M37" s="23">
+      <c r="M37" s="19">
         <v>2.06073584633384E-3</v>
       </c>
-      <c r="N37" s="23">
+      <c r="N37" s="19">
         <v>1.9087501730713E-3</v>
       </c>
-      <c r="O37" s="23">
+      <c r="O37" s="19">
         <v>1.76250606817293E-3</v>
       </c>
-      <c r="P37" s="23">
+      <c r="P37" s="19">
         <v>1.6213981693252999E-3</v>
       </c>
-      <c r="Q37" s="23">
+      <c r="Q37" s="19">
         <v>1.4849205588616399E-3</v>
       </c>
-      <c r="R37" s="23">
+      <c r="R37" s="19">
         <v>1.3526452932388501E-3</v>
       </c>
-      <c r="S37" s="23">
+      <c r="S37" s="19">
         <v>1.2242065486077001E-3</v>
       </c>
-      <c r="T37" s="23">
+      <c r="T37" s="19">
         <v>1.0992886850102899E-3</v>
       </c>
-      <c r="U37" s="23">
+      <c r="U37" s="19">
         <v>9.7761710668958801E-4</v>
       </c>
-      <c r="V37" s="23">
+      <c r="V37" s="19">
         <v>8.5895115730887496E-4</v>
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A38" s="22" t="s">
+      <c r="A38" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B38" s="23">
+      <c r="B38" s="19">
         <f>SUM(B36:B37)</f>
         <v>2.5943952966763138E-2</v>
       </c>
-      <c r="C38" s="23">
+      <c r="C38" s="19">
         <f t="shared" ref="C38:V38" si="7">SUM(C36:C37)</f>
         <v>1.54636722038725E-2</v>
       </c>
-      <c r="D38" s="23">
+      <c r="D38" s="19">
         <f t="shared" si="7"/>
         <v>9.2742473233851409E-3</v>
       </c>
-      <c r="E38" s="23">
+      <c r="E38" s="19">
         <f t="shared" si="7"/>
         <v>8.2884580787050896E-3</v>
       </c>
-      <c r="F38" s="23">
+      <c r="F38" s="19">
         <f t="shared" si="7"/>
         <v>5.3045012487175002E-3</v>
       </c>
-      <c r="G38" s="23">
+      <c r="G38" s="19">
         <f t="shared" si="7"/>
         <v>4.39753276850077E-3</v>
       </c>
-      <c r="H38" s="23">
+      <c r="H38" s="19">
         <f t="shared" si="7"/>
         <v>3.8031744028528902E-3</v>
       </c>
-      <c r="I38" s="23">
+      <c r="I38" s="19">
         <f t="shared" si="7"/>
         <v>3.4249250010206047E-3</v>
       </c>
-      <c r="J38" s="23">
+      <c r="J38" s="19">
         <f t="shared" si="7"/>
         <v>3.0300490707755069E-3</v>
       </c>
-      <c r="K38" s="23">
+      <c r="K38" s="19">
         <f t="shared" si="7"/>
         <v>2.750517818215462E-3</v>
       </c>
-      <c r="L38" s="23">
+      <c r="L38" s="19">
         <f t="shared" si="7"/>
         <v>2.5108708257625678E-3</v>
       </c>
-      <c r="M38" s="23">
+      <c r="M38" s="19">
         <f t="shared" si="7"/>
         <v>2.299372229839061E-3</v>
       </c>
-      <c r="N38" s="23">
+      <c r="N38" s="19">
         <f t="shared" si="7"/>
         <v>2.107345768743038E-3</v>
       </c>
-      <c r="O38" s="23">
+      <c r="O38" s="19">
         <f t="shared" si="7"/>
         <v>1.930939174205478E-3</v>
       </c>
-      <c r="P38" s="23">
+      <c r="P38" s="19">
         <f t="shared" si="7"/>
         <v>1.7665083615798229E-3</v>
       </c>
-      <c r="Q38" s="23">
+      <c r="Q38" s="19">
         <f t="shared" si="7"/>
         <v>1.611514314896446E-3</v>
       </c>
-      <c r="R38" s="23">
+      <c r="R38" s="19">
         <f t="shared" si="7"/>
         <v>1.464464244531832E-3</v>
       </c>
-      <c r="S38" s="23">
+      <c r="S38" s="19">
         <f t="shared" si="7"/>
         <v>1.3240858376809763E-3</v>
       </c>
-      <c r="T38" s="23">
+      <c r="T38" s="19">
         <f t="shared" si="7"/>
         <v>1.1894035666051008E-3</v>
       </c>
-      <c r="U38" s="23">
+      <c r="U38" s="19">
         <f t="shared" si="7"/>
         <v>1.0596098576443221E-3</v>
       </c>
-      <c r="V38" s="23">
+      <c r="V38" s="19">
         <f t="shared" si="7"/>
         <v>9.3408257734605728E-4</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A39" s="19"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
-      <c r="L39" s="20"/>
-      <c r="M39" s="20"/>
-      <c r="N39" s="20"/>
-      <c r="O39" s="20"/>
-      <c r="P39" s="20"/>
-      <c r="Q39" s="20"/>
-      <c r="R39" s="20"/>
-      <c r="S39" s="20"/>
-      <c r="T39" s="20"/>
-      <c r="U39" s="20"/>
-      <c r="V39" s="20"/>
+      <c r="A39" s="15"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="16"/>
+      <c r="N39" s="16"/>
+      <c r="O39" s="16"/>
+      <c r="P39" s="16"/>
+      <c r="Q39" s="16"/>
+      <c r="R39" s="16"/>
+      <c r="S39" s="16"/>
+      <c r="T39" s="16"/>
+      <c r="U39" s="16"/>
+      <c r="V39" s="16"/>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A40" s="22" t="s">
+      <c r="A40" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
-      <c r="L40" s="20"/>
-      <c r="M40" s="20"/>
-      <c r="N40" s="20"/>
-      <c r="O40" s="20"/>
-      <c r="P40" s="20"/>
-      <c r="Q40" s="20"/>
-      <c r="R40" s="20"/>
-      <c r="S40" s="20"/>
-      <c r="T40" s="20"/>
-      <c r="U40" s="20"/>
-      <c r="V40" s="20"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="16"/>
+      <c r="M40" s="16"/>
+      <c r="N40" s="16"/>
+      <c r="O40" s="16"/>
+      <c r="P40" s="16"/>
+      <c r="Q40" s="16"/>
+      <c r="R40" s="16"/>
+      <c r="S40" s="16"/>
+      <c r="T40" s="16"/>
+      <c r="U40" s="16"/>
+      <c r="V40" s="16"/>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="23">
+      <c r="B41" s="19">
         <v>1.7896825396825401E-3</v>
       </c>
-      <c r="C41" s="23">
+      <c r="C41" s="19">
         <v>1.7896825396825401E-3</v>
       </c>
-      <c r="D41" s="23">
+      <c r="D41" s="19">
         <v>1.7896825396825401E-3</v>
       </c>
-      <c r="E41" s="23">
+      <c r="E41" s="19">
         <v>1.7896825396825401E-3</v>
       </c>
-      <c r="F41" s="23">
+      <c r="F41" s="19">
         <v>1.7896825396825401E-3</v>
       </c>
-      <c r="G41" s="23">
+      <c r="G41" s="19">
         <v>1.7896825396825401E-3</v>
       </c>
-      <c r="H41" s="23">
+      <c r="H41" s="19">
         <v>1.7896825396825401E-3</v>
       </c>
-      <c r="I41" s="23">
+      <c r="I41" s="19">
         <v>1.7896825396825401E-3</v>
       </c>
-      <c r="J41" s="23">
+      <c r="J41" s="19">
         <v>1.7896825396825401E-3</v>
       </c>
-      <c r="K41" s="23">
+      <c r="K41" s="19">
         <v>1.7896825396825401E-3</v>
       </c>
-      <c r="L41" s="23">
+      <c r="L41" s="19">
         <v>1.7896825396825401E-3</v>
       </c>
-      <c r="M41" s="23">
+      <c r="M41" s="19">
         <v>1.7896825396825401E-3</v>
       </c>
-      <c r="N41" s="23">
+      <c r="N41" s="19">
         <v>1.7896825396825401E-3</v>
       </c>
-      <c r="O41" s="23">
+      <c r="O41" s="19">
         <v>1.7896825396825401E-3</v>
       </c>
-      <c r="P41" s="23">
+      <c r="P41" s="19">
         <v>1.7896825396825401E-3</v>
       </c>
-      <c r="Q41" s="23">
+      <c r="Q41" s="19">
         <v>1.7896825396825401E-3</v>
       </c>
-      <c r="R41" s="23">
+      <c r="R41" s="19">
         <v>1.7896825396825401E-3</v>
       </c>
-      <c r="S41" s="23">
+      <c r="S41" s="19">
         <v>1.7896825396825401E-3</v>
       </c>
-      <c r="T41" s="23">
+      <c r="T41" s="19">
         <v>1.7896825396825401E-3</v>
       </c>
-      <c r="U41" s="23">
+      <c r="U41" s="19">
         <v>1.7896825396825401E-3</v>
       </c>
-      <c r="V41" s="23">
+      <c r="V41" s="19">
         <v>1.7896825396825401E-3</v>
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="B42" s="25">
+      <c r="B42" s="21">
         <v>1.5E-3</v>
       </c>
-      <c r="C42" s="25">
+      <c r="C42" s="21">
         <v>1.5E-3</v>
       </c>
-      <c r="D42" s="25">
+      <c r="D42" s="21">
         <v>1.5E-3</v>
       </c>
-      <c r="E42" s="25">
+      <c r="E42" s="21">
         <v>1.5E-3</v>
       </c>
-      <c r="F42" s="25">
+      <c r="F42" s="21">
         <v>1.5E-3</v>
       </c>
-      <c r="G42" s="25">
+      <c r="G42" s="21">
         <v>1.5E-3</v>
       </c>
-      <c r="H42" s="25">
+      <c r="H42" s="21">
         <v>1.5E-3</v>
       </c>
-      <c r="I42" s="25">
+      <c r="I42" s="21">
         <v>1.5E-3</v>
       </c>
-      <c r="J42" s="25">
+      <c r="J42" s="21">
         <v>1.5E-3</v>
       </c>
-      <c r="K42" s="25">
+      <c r="K42" s="21">
         <v>1.5E-3</v>
       </c>
-      <c r="L42" s="25">
+      <c r="L42" s="21">
         <v>1.5E-3</v>
       </c>
-      <c r="M42" s="25">
+      <c r="M42" s="21">
         <v>1.5E-3</v>
       </c>
-      <c r="N42" s="25">
+      <c r="N42" s="21">
         <v>1.5E-3</v>
       </c>
-      <c r="O42" s="25">
+      <c r="O42" s="21">
         <v>1.5E-3</v>
       </c>
-      <c r="P42" s="25">
+      <c r="P42" s="21">
         <v>1.5E-3</v>
       </c>
-      <c r="Q42" s="25">
+      <c r="Q42" s="21">
         <v>1.5E-3</v>
       </c>
-      <c r="R42" s="25">
+      <c r="R42" s="21">
         <v>1.5E-3</v>
       </c>
-      <c r="S42" s="25">
+      <c r="S42" s="21">
         <v>1.5E-3</v>
       </c>
-      <c r="T42" s="25">
+      <c r="T42" s="21">
         <v>1.5E-3</v>
       </c>
-      <c r="U42" s="25">
+      <c r="U42" s="21">
         <v>1.5E-3</v>
       </c>
-      <c r="V42" s="25">
+      <c r="V42" s="21">
         <v>1.5E-3</v>
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A43" s="19" t="s">
+      <c r="A43" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="B43" s="23">
+      <c r="B43" s="19">
         <v>1.94137806637807E-3</v>
       </c>
-      <c r="C43" s="23">
+      <c r="C43" s="19">
         <v>1.94137806637807E-3</v>
       </c>
-      <c r="D43" s="23">
+      <c r="D43" s="19">
         <v>1.94137806637807E-3</v>
       </c>
-      <c r="E43" s="23">
+      <c r="E43" s="19">
         <v>1.94137806637807E-3</v>
       </c>
-      <c r="F43" s="23">
+      <c r="F43" s="19">
         <v>1.94137806637807E-3</v>
       </c>
-      <c r="G43" s="23">
+      <c r="G43" s="19">
         <v>1.94137806637807E-3</v>
       </c>
-      <c r="H43" s="23">
+      <c r="H43" s="19">
         <v>1.94137806637807E-3</v>
       </c>
-      <c r="I43" s="23">
+      <c r="I43" s="19">
         <v>1.94137806637807E-3</v>
       </c>
-      <c r="J43" s="23">
+      <c r="J43" s="19">
         <v>1.94137806637807E-3</v>
       </c>
-      <c r="K43" s="23">
+      <c r="K43" s="19">
         <v>1.94137806637807E-3</v>
       </c>
-      <c r="L43" s="23">
+      <c r="L43" s="19">
         <v>1.94137806637807E-3</v>
       </c>
-      <c r="M43" s="23">
+      <c r="M43" s="19">
         <v>1.94137806637807E-3</v>
       </c>
-      <c r="N43" s="23">
+      <c r="N43" s="19">
         <v>1.94137806637807E-3</v>
       </c>
-      <c r="O43" s="23">
+      <c r="O43" s="19">
         <v>1.94137806637807E-3</v>
       </c>
-      <c r="P43" s="23">
+      <c r="P43" s="19">
         <v>1.94137806637807E-3</v>
       </c>
-      <c r="Q43" s="23">
+      <c r="Q43" s="19">
         <v>1.94137806637807E-3</v>
       </c>
-      <c r="R43" s="23">
+      <c r="R43" s="19">
         <v>1.94137806637807E-3</v>
       </c>
-      <c r="S43" s="23">
+      <c r="S43" s="19">
         <v>1.94137806637807E-3</v>
       </c>
-      <c r="T43" s="23">
+      <c r="T43" s="19">
         <v>1.94137806637807E-3</v>
       </c>
-      <c r="U43" s="23">
+      <c r="U43" s="19">
         <v>1.94137806637807E-3</v>
       </c>
-      <c r="V43" s="23">
+      <c r="V43" s="19">
         <v>1.94137806637807E-3</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A44" s="19"/>
-      <c r="B44" s="23"/>
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="23"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
-      <c r="K44" s="23"/>
-      <c r="L44" s="23"/>
-      <c r="M44" s="23"/>
-      <c r="N44" s="23"/>
-      <c r="O44" s="23"/>
-      <c r="P44" s="23"/>
-      <c r="Q44" s="23"/>
-      <c r="R44" s="23"/>
-      <c r="S44" s="23"/>
-      <c r="T44" s="23"/>
-      <c r="U44" s="23"/>
-      <c r="V44" s="23"/>
+      <c r="A44" s="15"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="19"/>
+      <c r="L44" s="19"/>
+      <c r="M44" s="19"/>
+      <c r="N44" s="19"/>
+      <c r="O44" s="19"/>
+      <c r="P44" s="19"/>
+      <c r="Q44" s="19"/>
+      <c r="R44" s="19"/>
+      <c r="S44" s="19"/>
+      <c r="T44" s="19"/>
+      <c r="U44" s="19"/>
+      <c r="V44" s="19"/>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A45" s="22"/>
-      <c r="B45" s="23"/>
-      <c r="C45" s="23"/>
-      <c r="D45" s="23"/>
-      <c r="E45" s="23"/>
-      <c r="F45" s="23"/>
-      <c r="G45" s="23"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="23"/>
-      <c r="K45" s="23"/>
-      <c r="L45" s="23"/>
-      <c r="M45" s="23"/>
-      <c r="N45" s="23"/>
-      <c r="O45" s="23"/>
-      <c r="P45" s="23"/>
-      <c r="Q45" s="23"/>
-      <c r="R45" s="23"/>
-      <c r="S45" s="23"/>
-      <c r="T45" s="23"/>
-      <c r="U45" s="23"/>
-      <c r="V45" s="23"/>
+      <c r="A45" s="18"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
+      <c r="K45" s="19"/>
+      <c r="L45" s="19"/>
+      <c r="M45" s="19"/>
+      <c r="N45" s="19"/>
+      <c r="O45" s="19"/>
+      <c r="P45" s="19"/>
+      <c r="Q45" s="19"/>
+      <c r="R45" s="19"/>
+      <c r="S45" s="19"/>
+      <c r="T45" s="19"/>
+      <c r="U45" s="19"/>
+      <c r="V45" s="19"/>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A46" s="19" t="s">
+      <c r="A46" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B46" s="23">
+      <c r="B46" s="19">
         <v>1.29719764833815E-3</v>
       </c>
-      <c r="C46" s="23">
+      <c r="C46" s="19">
         <v>7.7318361019362305E-4</v>
       </c>
-      <c r="D46" s="23">
+      <c r="D46" s="19">
         <v>4.6371236616925699E-4</v>
       </c>
-      <c r="E46" s="23">
+      <c r="E46" s="19">
         <v>4.1442290393525402E-4</v>
       </c>
-      <c r="F46" s="23">
+      <c r="F46" s="19">
         <v>2.65225062435875E-4</v>
       </c>
-      <c r="G46" s="23">
+      <c r="G46" s="19">
         <v>2.1987663842503799E-4</v>
       </c>
-      <c r="H46" s="23">
+      <c r="H46" s="19">
         <v>1.9015872014264501E-4</v>
       </c>
-      <c r="I46" s="23">
+      <c r="I46" s="19">
         <v>1.7124625005102999E-4</v>
       </c>
-      <c r="J46" s="23">
+      <c r="J46" s="19">
         <v>1.5150245353877601E-4</v>
       </c>
-      <c r="K46" s="23">
+      <c r="K46" s="19">
         <v>1.3752589091077299E-4</v>
       </c>
-      <c r="L46" s="23">
+      <c r="L46" s="19">
         <v>1.25543541288128E-4</v>
       </c>
-      <c r="M46" s="23">
+      <c r="M46" s="19">
         <v>1.1496861149195299E-4</v>
       </c>
-      <c r="N46" s="23">
+      <c r="N46" s="19">
         <v>1.0536728843715199E-4</v>
       </c>
-      <c r="O46" s="23">
+      <c r="O46" s="19">
         <v>9.65469587102738E-5</v>
       </c>
-      <c r="P46" s="23">
+      <c r="P46" s="19">
         <v>8.8325418078991097E-5</v>
       </c>
-      <c r="Q46" s="23">
+      <c r="Q46" s="19">
         <v>8.0575715744822304E-5</v>
       </c>
-      <c r="R46" s="23">
+      <c r="R46" s="19">
         <v>7.3223212226591607E-5</v>
       </c>
-      <c r="S46" s="23">
+      <c r="S46" s="19">
         <v>6.6204291884049E-5</v>
       </c>
-      <c r="T46" s="23">
+      <c r="T46" s="19">
         <v>5.9470178330254899E-5</v>
       </c>
-      <c r="U46" s="23">
+      <c r="U46" s="19">
         <v>5.2980492882216097E-5</v>
       </c>
-      <c r="V46" s="23">
+      <c r="V46" s="19">
         <v>4.6704128867302902E-5</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="B47" s="23">
+      <c r="B47" s="19">
         <v>8.0513663447125095E-4</v>
       </c>
-      <c r="C47" s="23">
+      <c r="C47" s="19">
         <v>8.0513663447125095E-4</v>
       </c>
-      <c r="D47" s="23">
+      <c r="D47" s="19">
         <v>8.0513663447125095E-4</v>
       </c>
-      <c r="E47" s="23">
+      <c r="E47" s="19">
         <v>8.0513663447125095E-4</v>
       </c>
-      <c r="F47" s="23">
+      <c r="F47" s="19">
         <v>8.0513663447125095E-4</v>
       </c>
-      <c r="G47" s="23">
+      <c r="G47" s="19">
         <v>8.0513663447125095E-4</v>
       </c>
-      <c r="H47" s="23">
+      <c r="H47" s="19">
         <v>8.0513663447125095E-4</v>
       </c>
-      <c r="I47" s="23">
+      <c r="I47" s="19">
         <v>8.0513663447125095E-4</v>
       </c>
-      <c r="J47" s="23">
+      <c r="J47" s="19">
         <v>8.0513663447125095E-4</v>
       </c>
-      <c r="K47" s="23">
+      <c r="K47" s="19">
         <v>8.0513663447125095E-4</v>
       </c>
-      <c r="L47" s="23">
+      <c r="L47" s="19">
         <v>8.0513663447125095E-4</v>
       </c>
-      <c r="M47" s="23">
+      <c r="M47" s="19">
         <v>8.0513663447125095E-4</v>
       </c>
-      <c r="N47" s="23">
+      <c r="N47" s="19">
         <v>8.0513663447125095E-4</v>
       </c>
-      <c r="O47" s="23">
+      <c r="O47" s="19">
         <v>8.0513663447125095E-4</v>
       </c>
-      <c r="P47" s="23">
+      <c r="P47" s="19">
         <v>8.0513663447125095E-4</v>
       </c>
-      <c r="Q47" s="23">
+      <c r="Q47" s="19">
         <v>8.0513663447125095E-4</v>
       </c>
-      <c r="R47" s="23">
+      <c r="R47" s="19">
         <v>8.0513663447125095E-4</v>
       </c>
-      <c r="S47" s="23">
+      <c r="S47" s="19">
         <v>8.0513663447125095E-4</v>
       </c>
-      <c r="T47" s="23">
+      <c r="T47" s="19">
         <v>8.0513663447125095E-4</v>
       </c>
-      <c r="U47" s="23">
+      <c r="U47" s="19">
         <v>8.0513663447125095E-4</v>
       </c>
-      <c r="V47" s="23">
+      <c r="V47" s="19">
         <v>8.0513663447125095E-4</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A48" s="19" t="s">
+      <c r="A48" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="B48" s="23">
+      <c r="B48" s="19">
         <v>1.5435859642862999E-6</v>
       </c>
-      <c r="C48" s="23">
+      <c r="C48" s="19">
         <v>1.5435859642862999E-6</v>
       </c>
-      <c r="D48" s="23">
+      <c r="D48" s="19">
         <v>1.5435859642862999E-6</v>
       </c>
-      <c r="E48" s="23">
+      <c r="E48" s="19">
         <v>1.5435859642862999E-6</v>
       </c>
-      <c r="F48" s="23">
+      <c r="F48" s="19">
         <v>1.5435859642862999E-6</v>
       </c>
-      <c r="G48" s="23">
+      <c r="G48" s="19">
         <v>1.5435859642862999E-6</v>
       </c>
-      <c r="H48" s="23">
+      <c r="H48" s="19">
         <v>1.5435859642862999E-6</v>
       </c>
-      <c r="I48" s="23">
+      <c r="I48" s="19">
         <v>1.5435859642862999E-6</v>
       </c>
-      <c r="J48" s="23">
+      <c r="J48" s="19">
         <v>1.5435859642862999E-6</v>
       </c>
-      <c r="K48" s="23">
+      <c r="K48" s="19">
         <v>1.5435859642862999E-6</v>
       </c>
-      <c r="L48" s="23">
+      <c r="L48" s="19">
         <v>1.5435859642862999E-6</v>
       </c>
-      <c r="M48" s="23">
+      <c r="M48" s="19">
         <v>1.5435859642862999E-6</v>
       </c>
-      <c r="N48" s="23">
+      <c r="N48" s="19">
         <v>1.5435859642862999E-6</v>
       </c>
-      <c r="O48" s="23">
+      <c r="O48" s="19">
         <v>1.5435859642862999E-6</v>
       </c>
-      <c r="P48" s="23">
+      <c r="P48" s="19">
         <v>1.5435859642862999E-6</v>
       </c>
-      <c r="Q48" s="23">
+      <c r="Q48" s="19">
         <v>1.5435859642862999E-6</v>
       </c>
-      <c r="R48" s="23">
+      <c r="R48" s="19">
         <v>1.5435859642862999E-6</v>
       </c>
-      <c r="S48" s="23">
+      <c r="S48" s="19">
         <v>1.5435859642862999E-6</v>
       </c>
-      <c r="T48" s="23">
+      <c r="T48" s="19">
         <v>1.5435859642862999E-6</v>
       </c>
-      <c r="U48" s="23">
+      <c r="U48" s="19">
         <v>1.5435859642862999E-6</v>
       </c>
-      <c r="V48" s="23">
+      <c r="V48" s="19">
         <v>1.5435859642862999E-6</v>
       </c>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A49" s="19" t="s">
+      <c r="A49" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="B49" s="23">
+      <c r="B49" s="19">
         <v>4.3529956131946E-5</v>
       </c>
-      <c r="C49" s="23">
+      <c r="C49" s="19">
         <v>4.3529956131946E-5</v>
       </c>
-      <c r="D49" s="23">
+      <c r="D49" s="19">
         <v>4.3529956131946E-5</v>
       </c>
-      <c r="E49" s="23">
+      <c r="E49" s="19">
         <v>4.3529956131946E-5</v>
       </c>
-      <c r="F49" s="23">
+      <c r="F49" s="19">
         <v>4.3529956131946E-5</v>
       </c>
-      <c r="G49" s="23">
+      <c r="G49" s="19">
         <v>4.3529956131946E-5</v>
       </c>
-      <c r="H49" s="23">
+      <c r="H49" s="19">
         <v>4.3529956131946E-5</v>
       </c>
-      <c r="I49" s="23">
+      <c r="I49" s="19">
         <v>4.3529956131946E-5</v>
       </c>
-      <c r="J49" s="23">
+      <c r="J49" s="19">
         <v>4.3529956131946E-5</v>
       </c>
-      <c r="K49" s="23">
+      <c r="K49" s="19">
         <v>4.3529956131946E-5</v>
       </c>
-      <c r="L49" s="23">
+      <c r="L49" s="19">
         <v>4.3529956131946E-5</v>
       </c>
-      <c r="M49" s="23">
+      <c r="M49" s="19">
         <v>4.3529956131946E-5</v>
       </c>
-      <c r="N49" s="23">
+      <c r="N49" s="19">
         <v>4.3529956131946E-5</v>
       </c>
-      <c r="O49" s="23">
+      <c r="O49" s="19">
         <v>4.3529956131946E-5</v>
       </c>
-      <c r="P49" s="23">
+      <c r="P49" s="19">
         <v>4.3529956131946E-5</v>
       </c>
-      <c r="Q49" s="23">
+      <c r="Q49" s="19">
         <v>4.3529956131946E-5</v>
       </c>
-      <c r="R49" s="23">
+      <c r="R49" s="19">
         <v>4.3529956131946E-5</v>
       </c>
-      <c r="S49" s="23">
+      <c r="S49" s="19">
         <v>4.3529956131946E-5</v>
       </c>
-      <c r="T49" s="23">
+      <c r="T49" s="19">
         <v>4.3529956131946E-5</v>
       </c>
-      <c r="U49" s="23">
+      <c r="U49" s="19">
         <v>4.3529956131946E-5</v>
       </c>
-      <c r="V49" s="23">
+      <c r="V49" s="19">
         <v>4.3529956131946E-5</v>
       </c>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A50" s="22" t="s">
+      <c r="A50" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B50" s="23">
+      <c r="B50" s="19">
         <f>SUM(B46:B49)</f>
         <v>2.147407824905633E-3</v>
       </c>
-      <c r="C50" s="23">
+      <c r="C50" s="19">
         <f t="shared" ref="C50:V50" si="8">SUM(C46:C49)</f>
         <v>1.6233937867611065E-3</v>
       </c>
-      <c r="D50" s="23">
+      <c r="D50" s="19">
         <f t="shared" si="8"/>
         <v>1.3139225427367402E-3</v>
       </c>
-      <c r="E50" s="23">
+      <c r="E50" s="19">
         <f t="shared" si="8"/>
         <v>1.2646330805027373E-3</v>
       </c>
-      <c r="F50" s="23">
+      <c r="F50" s="19">
         <f t="shared" si="8"/>
         <v>1.1154352390033582E-3</v>
       </c>
-      <c r="G50" s="23">
+      <c r="G50" s="19">
         <f t="shared" si="8"/>
         <v>1.0700868149925212E-3</v>
       </c>
-      <c r="H50" s="23">
+      <c r="H50" s="19">
         <f t="shared" si="8"/>
         <v>1.0403688967101283E-3</v>
       </c>
-      <c r="I50" s="23">
+      <c r="I50" s="19">
         <f t="shared" si="8"/>
         <v>1.0214564266185133E-3</v>
       </c>
-      <c r="J50" s="23">
+      <c r="J50" s="19">
         <f t="shared" si="8"/>
         <v>1.0017126301062594E-3</v>
       </c>
-      <c r="K50" s="23">
+      <c r="K50" s="19">
         <f t="shared" si="8"/>
         <v>9.8773606747825618E-4</v>
       </c>
-      <c r="L50" s="23">
+      <c r="L50" s="19">
         <f t="shared" si="8"/>
         <v>9.7575371785561132E-4</v>
       </c>
-      <c r="M50" s="23">
+      <c r="M50" s="19">
         <f t="shared" si="8"/>
         <v>9.6517878805943631E-4</v>
       </c>
-      <c r="N50" s="23">
+      <c r="N50" s="19">
         <f t="shared" si="8"/>
         <v>9.5557746500463526E-4</v>
       </c>
-      <c r="O50" s="23">
+      <c r="O50" s="19">
         <f t="shared" si="8"/>
         <v>9.467571352777571E-4</v>
       </c>
-      <c r="P50" s="23">
+      <c r="P50" s="19">
         <f t="shared" si="8"/>
         <v>9.3853559464647442E-4</v>
       </c>
-      <c r="Q50" s="23">
+      <c r="Q50" s="19">
         <f t="shared" si="8"/>
         <v>9.3078589231230559E-4</v>
       </c>
-      <c r="R50" s="23">
+      <c r="R50" s="19">
         <f t="shared" si="8"/>
         <v>9.2343338879407493E-4</v>
       </c>
-      <c r="S50" s="23">
+      <c r="S50" s="19">
         <f t="shared" si="8"/>
         <v>9.1641446845153228E-4</v>
       </c>
-      <c r="T50" s="23">
+      <c r="T50" s="19">
         <f t="shared" si="8"/>
         <v>9.0968035489773821E-4</v>
       </c>
-      <c r="U50" s="23">
+      <c r="U50" s="19">
         <f t="shared" si="8"/>
         <v>9.0319066944969935E-4</v>
       </c>
-      <c r="V50" s="23">
+      <c r="V50" s="19">
         <f t="shared" si="8"/>
         <v>8.9691430543478614E-4</v>
       </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A51" s="19"/>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
-      <c r="I51" s="20"/>
-      <c r="J51" s="20"/>
-      <c r="K51" s="20"/>
-      <c r="L51" s="20"/>
-      <c r="M51" s="20"/>
-      <c r="N51" s="20"/>
-      <c r="O51" s="20"/>
-      <c r="P51" s="20"/>
-      <c r="Q51" s="20"/>
-      <c r="R51" s="20"/>
-      <c r="S51" s="20"/>
-      <c r="T51" s="20"/>
-      <c r="U51" s="20"/>
-      <c r="V51" s="20"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="16"/>
+      <c r="H51" s="16"/>
+      <c r="I51" s="16"/>
+      <c r="J51" s="16"/>
+      <c r="K51" s="16"/>
+      <c r="L51" s="16"/>
+      <c r="M51" s="16"/>
+      <c r="N51" s="16"/>
+      <c r="O51" s="16"/>
+      <c r="P51" s="16"/>
+      <c r="Q51" s="16"/>
+      <c r="R51" s="16"/>
+      <c r="S51" s="16"/>
+      <c r="T51" s="16"/>
+      <c r="U51" s="16"/>
+      <c r="V51" s="16"/>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A52" s="22" t="s">
+      <c r="A52" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="B52" s="23">
+      <c r="B52" s="19">
         <v>1.825E-3</v>
       </c>
-      <c r="C52" s="23">
+      <c r="C52" s="19">
         <v>1.7702499999999999E-3</v>
       </c>
-      <c r="D52" s="23">
+      <c r="D52" s="19">
         <v>1.7155E-3</v>
       </c>
-      <c r="E52" s="23">
+      <c r="E52" s="19">
         <v>1.6607499999999999E-3</v>
       </c>
-      <c r="F52" s="23">
+      <c r="F52" s="19">
         <v>1.606E-3</v>
       </c>
-      <c r="G52" s="23">
+      <c r="G52" s="19">
         <v>1.5512499999999999E-3</v>
       </c>
-      <c r="H52" s="23">
+      <c r="H52" s="19">
         <v>1.4965E-3</v>
       </c>
-      <c r="I52" s="23">
+      <c r="I52" s="19">
         <v>1.4417500000000001E-3</v>
       </c>
-      <c r="J52" s="23">
+      <c r="J52" s="19">
         <v>1.387E-3</v>
       </c>
-      <c r="K52" s="23">
+      <c r="K52" s="19">
         <v>1.3322500000000001E-3</v>
       </c>
-      <c r="L52" s="23">
+      <c r="L52" s="19">
         <v>1.2775E-3</v>
       </c>
-      <c r="M52" s="23">
+      <c r="M52" s="19">
         <v>1.2227500000000001E-3</v>
       </c>
-      <c r="N52" s="23">
+      <c r="N52" s="19">
         <v>1.168E-3</v>
       </c>
-      <c r="O52" s="23">
+      <c r="O52" s="19">
         <v>1.1132500000000001E-3</v>
       </c>
-      <c r="P52" s="23">
+      <c r="P52" s="19">
         <v>1.0585E-3</v>
       </c>
-      <c r="Q52" s="23">
+      <c r="Q52" s="19">
         <v>1.0037500000000001E-3</v>
       </c>
-      <c r="R52" s="23">
+      <c r="R52" s="19">
         <v>9.4899999999999997E-4</v>
       </c>
-      <c r="S52" s="23">
+      <c r="S52" s="19">
         <v>8.9424999999999997E-4</v>
       </c>
-      <c r="T52" s="23">
+      <c r="T52" s="19">
         <v>8.3949999999999997E-4</v>
       </c>
-      <c r="U52" s="23">
+      <c r="U52" s="19">
         <v>7.8474999999999997E-4</v>
       </c>
-      <c r="V52" s="23">
+      <c r="V52" s="19">
         <v>7.2999999999999996E-4</v>
       </c>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A53" s="20"/>
-      <c r="B53" s="20"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
-      <c r="G53" s="20"/>
-      <c r="H53" s="20"/>
-      <c r="I53" s="20"/>
-      <c r="J53" s="20"/>
-      <c r="K53" s="20"/>
-      <c r="L53" s="20"/>
-      <c r="M53" s="20"/>
-      <c r="N53" s="20"/>
-      <c r="O53" s="20"/>
-      <c r="P53" s="20"/>
-      <c r="Q53" s="20"/>
-      <c r="R53" s="20"/>
-      <c r="S53" s="20"/>
-      <c r="T53" s="20"/>
-      <c r="U53" s="20"/>
-      <c r="V53" s="20"/>
+      <c r="A53" s="16"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16"/>
+      <c r="I53" s="16"/>
+      <c r="J53" s="16"/>
+      <c r="K53" s="16"/>
+      <c r="L53" s="16"/>
+      <c r="M53" s="16"/>
+      <c r="N53" s="16"/>
+      <c r="O53" s="16"/>
+      <c r="P53" s="16"/>
+      <c r="Q53" s="16"/>
+      <c r="R53" s="16"/>
+      <c r="S53" s="16"/>
+      <c r="T53" s="16"/>
+      <c r="U53" s="16"/>
+      <c r="V53" s="16"/>
     </row>
     <row r="54" spans="1:23" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="27" t="s">
+      <c r="A54" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="B54" s="28">
+      <c r="B54" s="24">
         <f t="shared" ref="B54:V54" si="9">SUM(B24:B25,B27:B28,B36:B37,B41:B43,B46:B49,B52)</f>
         <v>0.11509588998916793</v>
       </c>
-      <c r="C54" s="28">
+      <c r="C54" s="24">
         <f t="shared" si="9"/>
         <v>9.4026411153444484E-2</v>
       </c>
-      <c r="D54" s="28">
+      <c r="D54" s="24">
         <f t="shared" si="9"/>
         <v>6.1030347880098958E-2</v>
       </c>
-      <c r="E54" s="28">
+      <c r="E54" s="24">
         <f t="shared" si="9"/>
         <v>4.5988209401186815E-2</v>
       </c>
-      <c r="F54" s="28">
+      <c r="F54" s="24">
         <f t="shared" si="9"/>
         <v>3.4845175121645797E-2</v>
       </c>
-      <c r="G54" s="28">
+      <c r="G54" s="24">
         <f t="shared" si="9"/>
         <v>2.9884949141511838E-2</v>
       </c>
-      <c r="H54" s="28">
+      <c r="H54" s="24">
         <f t="shared" si="9"/>
         <v>2.690006260060478E-2</v>
       </c>
-      <c r="I54" s="28">
+      <c r="I54" s="24">
         <f t="shared" si="9"/>
         <v>2.5054989871554936E-2</v>
       </c>
-      <c r="J54" s="28">
+      <c r="J54" s="24">
         <f t="shared" si="9"/>
         <v>2.3699600577761132E-2</v>
       </c>
-      <c r="K54" s="28">
+      <c r="K54" s="24">
         <f t="shared" si="9"/>
         <v>2.268882456735534E-2</v>
       </c>
-      <c r="L54" s="28">
+      <c r="L54" s="24">
         <f t="shared" si="9"/>
         <v>2.1904754143909445E-2</v>
       </c>
-      <c r="M54" s="28">
+      <c r="M54" s="24">
         <f t="shared" si="9"/>
         <v>2.1266279860766003E-2</v>
       </c>
-      <c r="N54" s="28">
+      <c r="N54" s="24">
         <f t="shared" si="9"/>
         <v>2.0745315228228367E-2</v>
       </c>
-      <c r="O54" s="28">
+      <c r="O54" s="24">
         <f t="shared" si="9"/>
         <v>2.0312659395549462E-2</v>
       </c>
-      <c r="P54" s="28">
+      <c r="P54" s="24">
         <f t="shared" si="9"/>
         <v>1.992888418152159E-2</v>
       </c>
-      <c r="Q54" s="28">
+      <c r="Q54" s="24">
         <f t="shared" si="9"/>
         <v>1.9600450333245485E-2</v>
       </c>
-      <c r="R54" s="28">
+      <c r="R54" s="24">
         <f t="shared" si="9"/>
         <v>1.9307806745871618E-2</v>
       </c>
-      <c r="S54" s="28">
+      <c r="S54" s="24">
         <f t="shared" si="9"/>
         <v>1.9054607648030568E-2</v>
       </c>
-      <c r="T54" s="28">
+      <c r="T54" s="24">
         <f t="shared" si="9"/>
         <v>1.880114261962465E-2</v>
       </c>
-      <c r="U54" s="28">
+      <c r="U54" s="24">
         <f t="shared" si="9"/>
         <v>1.8583052649352855E-2</v>
       </c>
-      <c r="V54" s="28">
+      <c r="V54" s="24">
         <f t="shared" si="9"/>
         <v>1.8366902201183737E-2</v>
       </c>
-      <c r="W54" s="29" t="s">
+      <c r="W54" s="25" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="55" spans="1:23" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="27" t="s">
+      <c r="A55" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="B55" s="28">
+      <c r="B55" s="24">
         <f>SUM(B24:B25,B27:B28,B36:B37,B42:B43,B46:B49,B52)</f>
         <v>0.1133062074494854</v>
       </c>
-      <c r="C55" s="28">
+      <c r="C55" s="24">
         <f t="shared" ref="C55:V55" si="10">SUM(C24:C25,C27:C28,C36:C37,C42:C43,C46:C49,C52)</f>
         <v>9.2236728613761948E-2</v>
       </c>
-      <c r="D55" s="28">
+      <c r="D55" s="24">
         <f t="shared" si="10"/>
         <v>5.9240665340416415E-2</v>
       </c>
-      <c r="E55" s="28">
+      <c r="E55" s="24">
         <f t="shared" si="10"/>
         <v>4.4198526861504273E-2</v>
       </c>
-      <c r="F55" s="28">
+      <c r="F55" s="24">
         <f t="shared" si="10"/>
         <v>3.3055492581963254E-2</v>
       </c>
-      <c r="G55" s="28">
+      <c r="G55" s="24">
         <f t="shared" si="10"/>
         <v>2.8095266601829299E-2</v>
       </c>
-      <c r="H55" s="28">
+      <c r="H55" s="24">
         <f t="shared" si="10"/>
         <v>2.5110380060922241E-2</v>
       </c>
-      <c r="I55" s="28">
+      <c r="I55" s="24">
         <f t="shared" si="10"/>
         <v>2.3265307331872397E-2</v>
       </c>
-      <c r="J55" s="28">
+      <c r="J55" s="24">
         <f t="shared" si="10"/>
         <v>2.1909918038078593E-2</v>
       </c>
-      <c r="K55" s="28">
+      <c r="K55" s="24">
         <f t="shared" si="10"/>
         <v>2.0899142027672801E-2</v>
       </c>
-      <c r="L55" s="28">
+      <c r="L55" s="24">
         <f t="shared" si="10"/>
         <v>2.0115071604226906E-2</v>
       </c>
-      <c r="M55" s="28">
+      <c r="M55" s="24">
         <f t="shared" si="10"/>
         <v>1.947659732108346E-2</v>
       </c>
-      <c r="N55" s="28">
+      <c r="N55" s="24">
         <f t="shared" si="10"/>
         <v>1.8955632688545825E-2</v>
       </c>
-      <c r="O55" s="28">
+      <c r="O55" s="24">
         <f t="shared" si="10"/>
         <v>1.8522976855866919E-2</v>
       </c>
-      <c r="P55" s="28">
+      <c r="P55" s="24">
         <f t="shared" si="10"/>
         <v>1.8139201641839048E-2</v>
       </c>
-      <c r="Q55" s="28">
+      <c r="Q55" s="24">
         <f t="shared" si="10"/>
         <v>1.7810767793562943E-2</v>
       </c>
-      <c r="R55" s="28">
+      <c r="R55" s="24">
         <f t="shared" si="10"/>
         <v>1.7518124206189079E-2</v>
       </c>
-      <c r="S55" s="28">
+      <c r="S55" s="24">
         <f t="shared" si="10"/>
         <v>1.7264925108348025E-2</v>
       </c>
-      <c r="T55" s="28">
+      <c r="T55" s="24">
         <f t="shared" si="10"/>
         <v>1.7011460079942108E-2</v>
       </c>
-      <c r="U55" s="28">
+      <c r="U55" s="24">
         <f t="shared" si="10"/>
         <v>1.6793370109670313E-2</v>
       </c>
-      <c r="V55" s="28">
+      <c r="V55" s="24">
         <f t="shared" si="10"/>
         <v>1.6577219661501195E-2</v>
       </c>
-      <c r="W55" s="29" t="s">
+      <c r="W55" s="25" t="s">
         <v>105</v>
       </c>
     </row>
@@ -6284,7 +6350,7 @@
       </c>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A60" s="18" t="s">
+      <c r="A60" s="14" t="s">
         <v>77</v>
       </c>
       <c r="B60" s="1">
@@ -6373,7 +6439,7 @@
       </c>
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A61" s="18" t="s">
+      <c r="A61" s="14" t="s">
         <v>76</v>
       </c>
       <c r="B61" s="1">

</xml_diff>

<commit_message>
made another folder for sizing
</commit_message>
<xml_diff>
--- a/Wing Tail Drag Buildup/Drag.xlsx
+++ b/Wing Tail Drag Buildup/Drag.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EddieH\Documents\GitHub\Senior-Design\Wing Tail Drag Buildup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8D1D27-429B-45E1-ACE9-FD900AE7469A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E458632-1FCC-412C-9562-8F1A203410A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2768" yWindow="1500" windowWidth="22201" windowHeight="13605" xr2:uid="{82617F0D-A785-403D-9CC0-085A46D2A0AD}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{82617F0D-A785-403D-9CC0-085A46D2A0AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3708,8 +3708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470D6C11-8322-4BAC-B928-8395D64AAF23}">
   <dimension ref="A1:W61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4393,7 +4393,7 @@
         <v>1.5</v>
       </c>
       <c r="C23" s="19">
-        <f t="shared" ref="C23:V23" si="3" xml:space="preserve"> $D$6/(0.5*$J$3*C21^2*$J$4)</f>
+        <f t="shared" ref="B23:V23" si="3" xml:space="preserve"> $D$6/(0.5*$J$3*C21^2*$J$4)</f>
         <v>1.4823406325816004</v>
       </c>
       <c r="D23" s="19">
@@ -4991,77 +4991,77 @@
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A31" s="15"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16"/>
-      <c r="K31" s="16"/>
-      <c r="L31" s="16"/>
-      <c r="M31" s="16"/>
-      <c r="N31" s="16"/>
-      <c r="O31" s="16"/>
-      <c r="P31" s="16"/>
-      <c r="Q31" s="16"/>
-      <c r="R31" s="16"/>
-      <c r="S31" s="16"/>
-      <c r="T31" s="16"/>
-      <c r="U31" s="16"/>
-      <c r="V31" s="16"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="15"/>
+      <c r="S31" s="15"/>
+      <c r="T31" s="15"/>
+      <c r="U31" s="15"/>
+      <c r="V31" s="15"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A32" s="15"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="16"/>
-      <c r="K32" s="16"/>
-      <c r="L32" s="16"/>
-      <c r="M32" s="16"/>
-      <c r="N32" s="16"/>
-      <c r="O32" s="16"/>
-      <c r="P32" s="16"/>
-      <c r="Q32" s="16"/>
-      <c r="R32" s="16"/>
-      <c r="S32" s="16"/>
-      <c r="T32" s="16"/>
-      <c r="U32" s="16"/>
-      <c r="V32" s="16"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="15"/>
+      <c r="S32" s="15"/>
+      <c r="T32" s="15"/>
+      <c r="U32" s="15"/>
+      <c r="V32" s="15"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A33" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="16"/>
-      <c r="K33" s="16"/>
-      <c r="L33" s="16"/>
-      <c r="M33" s="16"/>
-      <c r="N33" s="16"/>
-      <c r="O33" s="16"/>
-      <c r="P33" s="16"/>
-      <c r="Q33" s="16"/>
-      <c r="R33" s="16"/>
-      <c r="S33" s="16"/>
-      <c r="T33" s="16"/>
-      <c r="U33" s="16"/>
-      <c r="V33" s="16"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="15"/>
+      <c r="S33" s="15"/>
+      <c r="T33" s="15"/>
+      <c r="U33" s="15"/>
+      <c r="V33" s="15"/>
       <c r="W33" s="26"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.45">

</xml_diff>